<commit_message>
Update for Jan 31 data
</commit_message>
<xml_diff>
--- a/data/pandemic2020.xlsx
+++ b/data/pandemic2020.xlsx
@@ -6,12 +6,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43E856-74A7-7E47-895B-DC33807DC050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC2CE67-CD12-8A43-BBDB-BB70AC579C8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="460" windowWidth="31160" windowHeight="24140" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="3560" yWindow="6560" windowWidth="27060" windowHeight="20980" activeTab="3" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
           <c:yMode val="edge"/>
           <c:x val="6.5050183833836636E-2"/>
           <c:y val="7.5846714013689448E-2"/>
-          <c:w val="0.8320662133142448"/>
+          <c:w val="0.85933894058697224"/>
           <c:h val="0.83735898821470844"/>
         </c:manualLayout>
       </c:layout>
@@ -322,41 +322,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -364,38 +367,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$4:$E$14</c:f>
+              <c:f>data!$E$4:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>17988</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>15238</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>12167</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9239</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6973</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -436,41 +442,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -478,41 +487,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$4:$F$14</c:f>
+              <c:f>data!$F$4:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>11791</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9692</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>7711</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5974</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4515</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -553,41 +565,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -595,38 +610,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$4:$G$14</c:f>
+              <c:f>data!$G$4:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1527</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1370</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1239</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>976</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -667,41 +685,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -709,38 +730,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$4:$H$14</c:f>
+              <c:f>data!$H$4:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -794,7 +818,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1125,35 +1149,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$12</c:f>
+              <c:f>data!$U$4:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1161,35 +1188,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$X$4:$X$12</c:f>
+              <c:f>data!$X$4:$X$13</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3071</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2928</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2266</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1179</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>719</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>893</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>679</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>393</c:v>
                 </c:pt>
               </c:numCache>
@@ -1230,35 +1260,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$12</c:f>
+              <c:f>data!$U$4:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1266,35 +1299,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$Y$4:$Y$12</c:f>
+              <c:f>data!$Y$4:$Y$13</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2099</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1981</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1737</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1459</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1771</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>769</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>688</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>457</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
@@ -1335,35 +1371,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$12</c:f>
+              <c:f>data!$U$4:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1371,35 +1410,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$Z$4:$Z$12</c:f>
+              <c:f>data!$Z$4:$Z$13</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>263</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>137</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>87</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>-7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1440,35 +1482,38 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$12</c:f>
+              <c:f>data!$U$4:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1476,35 +1521,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AA$4:$AA$12</c:f>
+              <c:f>data!$AA$4:$AA$13</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1558,7 +1606,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1904,41 +1952,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -1946,38 +1997,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$4:$H$14</c:f>
+              <c:f>data!$H$4:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -2018,41 +2072,44 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$14</c:f>
+              <c:f>data!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>43861</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -2060,32 +2117,35 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$I$4:$I$14</c:f>
+              <c:f>data!$I$4:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>171</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>103</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
@@ -2139,7 +2199,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4422,10 +4482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B1:AB25"/>
+  <dimension ref="B1:AB26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4531,999 +4591,1090 @@
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="C4" s="3">
-        <v>113579</v>
+        <v>136987</v>
       </c>
       <c r="D4" s="3">
-        <v>102427</v>
+        <v>118478</v>
       </c>
       <c r="E4" s="3">
-        <v>15238</v>
+        <v>17988</v>
       </c>
       <c r="F4" s="3">
-        <v>9692</v>
+        <v>11791</v>
       </c>
       <c r="G4" s="3">
-        <v>1527</v>
+        <v>1795</v>
       </c>
       <c r="H4" s="3">
-        <v>213</v>
+        <v>259</v>
       </c>
       <c r="I4" s="3">
-        <v>171</v>
+        <v>243</v>
       </c>
       <c r="K4" s="1">
         <f>B4</f>
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="L4" s="4">
-        <f>IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.28058584104720774</v>
+        <f t="shared" ref="L4" si="0">IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
+        <v>0.20609443647153092</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" ref="M4" si="0">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.24991762968748099</v>
+        <f t="shared" ref="M4" si="1">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
+        <v>0.15670672771827743</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" ref="N4" si="1">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
-        <v>0.25240404372482939</v>
+        <f t="shared" ref="N4" si="2">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
+        <v>0.18046987793673708</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4" si="2">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
-        <v>0.25690571910258075</v>
+        <f t="shared" ref="O4" si="3">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
+        <v>0.21657036731324797</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" ref="P4" si="3">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
-        <v>0.11459854014598547</v>
+        <f t="shared" ref="P4" si="4">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
+        <v>0.17550753110674533</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:R4" si="4">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
-        <v>0.25294117647058822</v>
+        <f t="shared" ref="Q4" si="5">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
+        <v>0.215962441314554</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" si="4"/>
-        <v>0.37903225806451624</v>
+        <f t="shared" ref="R4" si="6">IF(ISERROR(I4/I5-1)=TRUE, "", I4/I5-1)</f>
+        <v>0.42105263157894735</v>
       </c>
       <c r="S4" s="5">
         <f>H4/F4</f>
-        <v>2.1976888155179529E-2</v>
+        <v>2.1965906199643795E-2</v>
       </c>
       <c r="U4" s="1">
         <f>K4</f>
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="V4" s="14">
         <f>C4-C5</f>
-        <v>24886</v>
+        <v>23408</v>
       </c>
       <c r="W4" s="14">
-        <f t="shared" ref="W4:AB4" si="5">D4-D5</f>
-        <v>20480</v>
+        <f t="shared" ref="W4" si="7">D4-D5</f>
+        <v>16051</v>
       </c>
       <c r="X4" s="14">
-        <f t="shared" si="5"/>
-        <v>3071</v>
+        <f t="shared" ref="X4" si="8">E4-E5</f>
+        <v>2750</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" si="5"/>
-        <v>1981</v>
+        <f t="shared" ref="Y4" si="9">F4-F5</f>
+        <v>2099</v>
       </c>
       <c r="Z4" s="14">
-        <f t="shared" si="5"/>
-        <v>157</v>
+        <f t="shared" ref="Z4" si="10">G4-G5</f>
+        <v>268</v>
       </c>
       <c r="AA4" s="14">
-        <f t="shared" si="5"/>
-        <v>43</v>
+        <f t="shared" ref="AA4" si="11">H4-H5</f>
+        <v>46</v>
       </c>
       <c r="AB4" s="14">
-        <f t="shared" si="5"/>
-        <v>47</v>
+        <f t="shared" ref="AB4" si="12">I4-I5</f>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43859</v>
+        <v>43860</v>
       </c>
       <c r="C5" s="3">
-        <v>88693</v>
+        <v>113579</v>
       </c>
       <c r="D5" s="3">
-        <v>81947</v>
+        <v>102427</v>
       </c>
       <c r="E5" s="3">
-        <v>12167</v>
+        <v>15238</v>
       </c>
       <c r="F5" s="3">
-        <v>7711</v>
+        <v>9692</v>
       </c>
       <c r="G5" s="3">
-        <v>1370</v>
+        <v>1527</v>
       </c>
       <c r="H5" s="3">
-        <v>170</v>
+        <v>213</v>
       </c>
       <c r="I5" s="3">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="K5" s="1">
         <f>B5</f>
-        <v>43859</v>
+        <v>43860</v>
       </c>
       <c r="L5" s="4">
-        <f>IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
-        <v>0.35332712818713086</v>
+        <f t="shared" ref="L5:L10" si="13">IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
+        <v>0.28058584104720774</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5" si="6">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
-        <v>0.36601100183363888</v>
+        <f t="shared" ref="M5" si="14">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.24991762968748099</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" ref="N5" si="7">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
-        <v>0.31691741530468676</v>
+        <f t="shared" ref="N5" si="15">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+        <v>0.25240404372482939</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O5" si="8">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
-        <v>0.2907599598259123</v>
+        <f t="shared" ref="O5" si="16">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+        <v>0.25690571910258075</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" ref="P5" si="9">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
-        <v>0.10573042776432606</v>
+        <f t="shared" ref="P5" si="17">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+        <v>0.11459854014598547</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5:R5" si="10">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
-        <v>0.28787878787878785</v>
+        <f t="shared" ref="Q5:R5" si="18">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+        <v>0.25294117647058822</v>
       </c>
       <c r="R5" s="4">
-        <f t="shared" si="10"/>
-        <v>0.20388349514563098</v>
+        <f t="shared" si="18"/>
+        <v>0.37903225806451624</v>
       </c>
       <c r="S5" s="5">
         <f>H5/F5</f>
-        <v>2.2046427181947867E-2</v>
+        <v>2.1976888155179529E-2</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" ref="U5:U14" si="11">K5</f>
-        <v>43859</v>
+        <f>K5</f>
+        <v>43860</v>
       </c>
       <c r="V5" s="14">
-        <f t="shared" ref="V5:V12" si="12">C5-C6</f>
-        <v>23156</v>
+        <f>C5-C6</f>
+        <v>24886</v>
       </c>
       <c r="W5" s="14">
-        <f t="shared" ref="W5:W12" si="13">D5-D6</f>
-        <v>21957</v>
+        <f t="shared" ref="W5:AB5" si="19">D5-D6</f>
+        <v>20480</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" ref="X5:X12" si="14">E5-E6</f>
-        <v>2928</v>
+        <f t="shared" si="19"/>
+        <v>3071</v>
       </c>
       <c r="Y5" s="14">
-        <f t="shared" ref="Y5:Y12" si="15">F5-F6</f>
-        <v>1737</v>
+        <f t="shared" si="19"/>
+        <v>1981</v>
       </c>
       <c r="Z5" s="14">
-        <f t="shared" ref="Z5:Z12" si="16">G5-G6</f>
-        <v>131</v>
+        <f t="shared" si="19"/>
+        <v>157</v>
       </c>
       <c r="AA5" s="14">
-        <f t="shared" ref="AA5:AA12" si="17">H5-H6</f>
-        <v>38</v>
+        <f t="shared" si="19"/>
+        <v>43</v>
       </c>
       <c r="AB5" s="14">
-        <f t="shared" ref="AB5:AB12" si="18">I5-I6</f>
-        <v>21</v>
+        <f t="shared" si="19"/>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="C6" s="3">
-        <v>65537</v>
+        <v>88693</v>
       </c>
       <c r="D6" s="3">
-        <v>59990</v>
+        <v>81947</v>
       </c>
       <c r="E6" s="3">
-        <v>9239</v>
+        <v>12167</v>
       </c>
       <c r="F6" s="3">
-        <v>5974</v>
+        <v>7711</v>
       </c>
       <c r="G6" s="3">
-        <v>1239</v>
+        <v>1370</v>
       </c>
       <c r="H6" s="3">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="I6" s="3">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K6" s="1">
         <f>B6</f>
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="L6" s="4">
-        <f>IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
-        <v>0.37012104613969443</v>
+        <f t="shared" si="13"/>
+        <v>0.35332712818713086</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6" si="19">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
-        <v>0.35933109761624227</v>
+        <f t="shared" ref="M6" si="20">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
+        <v>0.36601100183363888</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6" si="20">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
-        <v>0.32496773268320656</v>
+        <f t="shared" ref="N6" si="21">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
+        <v>0.31691741530468676</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" ref="O6" si="21">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
-        <v>0.32314507198228126</v>
+        <f t="shared" ref="O6" si="22">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
+        <v>0.2907599598259123</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" ref="P6" si="22">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
-        <v>0.26946721311475419</v>
+        <f t="shared" ref="P6" si="23">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
+        <v>0.10573042776432606</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" ref="Q6:R6" si="23">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
-        <v>0.24528301886792447</v>
+        <f t="shared" ref="Q6:R6" si="24">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
+        <v>0.28787878787878785</v>
       </c>
       <c r="R6" s="4">
-        <f t="shared" si="23"/>
-        <v>0.71666666666666656</v>
+        <f t="shared" si="24"/>
+        <v>0.20388349514563098</v>
       </c>
       <c r="S6" s="5">
         <f>H6/F6</f>
-        <v>2.2095748242383664E-2</v>
+        <v>2.2046427181947867E-2</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="11"/>
-        <v>43858</v>
+        <f t="shared" ref="U6:U15" si="25">K6</f>
+        <v>43859</v>
       </c>
       <c r="V6" s="14">
-        <f t="shared" si="12"/>
-        <v>17704</v>
+        <f t="shared" ref="V6:V13" si="26">C6-C7</f>
+        <v>23156</v>
       </c>
       <c r="W6" s="14">
-        <f t="shared" si="13"/>
-        <v>15858</v>
+        <f t="shared" ref="W6:W13" si="27">D6-D7</f>
+        <v>21957</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" si="14"/>
-        <v>2266</v>
+        <f t="shared" ref="X6:X13" si="28">E6-E7</f>
+        <v>2928</v>
       </c>
       <c r="Y6" s="14">
-        <f t="shared" si="15"/>
-        <v>1459</v>
+        <f t="shared" ref="Y6:Y13" si="29">F6-F7</f>
+        <v>1737</v>
       </c>
       <c r="Z6" s="14">
-        <f t="shared" si="16"/>
-        <v>263</v>
+        <f t="shared" ref="Z6:Z13" si="30">G6-G7</f>
+        <v>131</v>
       </c>
       <c r="AA6" s="14">
-        <f t="shared" si="17"/>
-        <v>26</v>
+        <f t="shared" ref="AA6:AA13" si="31">H6-H7</f>
+        <v>38</v>
       </c>
       <c r="AB6" s="14">
-        <f t="shared" si="18"/>
-        <v>43</v>
+        <f t="shared" ref="AB6:AB13" si="32">I6-I7</f>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="C7" s="3">
-        <v>47833</v>
+        <v>65537</v>
       </c>
       <c r="D7" s="3">
-        <v>44132</v>
+        <v>59990</v>
       </c>
       <c r="E7" s="3">
-        <v>6973</v>
+        <v>9239</v>
       </c>
       <c r="F7" s="3">
-        <v>4515</v>
+        <v>5974</v>
       </c>
       <c r="G7" s="3">
-        <v>976</v>
+        <v>1239</v>
       </c>
       <c r="H7" s="3">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="I7" s="3">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="K7" s="1">
         <f>B7</f>
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="L7" s="4">
-        <f>IF(ISERROR(C7/C8-1)=TRUE, "", C7/C8-1)</f>
-        <v>0.45836763315954765</v>
+        <f t="shared" si="13"/>
+        <v>0.37012104613969443</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" ref="M7" si="24">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
-        <v>0.44918398844120455</v>
+        <f t="shared" ref="M7" si="33">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
+        <v>0.35933109761624227</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" ref="N7" si="25">IF(ISERROR(E7/E8-1)=TRUE, "", E7/E8-1)</f>
-        <v>0.20348636520538488</v>
+        <f t="shared" ref="N7" si="34">IF(ISERROR(E7/E8-1)=TRUE, "", E7/E8-1)</f>
+        <v>0.32496773268320656</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" ref="O7" si="26">IF(ISERROR(F7/F8-1)=TRUE, "", F7/F8-1)</f>
-        <v>0.64540816326530615</v>
+        <f t="shared" ref="O7" si="35">IF(ISERROR(F7/F8-1)=TRUE, "", F7/F8-1)</f>
+        <v>0.32314507198228126</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" ref="P7" si="27">IF(ISERROR(G7/G8-1)=TRUE, "", G7/G8-1)</f>
-        <v>1.1171366594360088</v>
+        <f t="shared" ref="P7" si="36">IF(ISERROR(G7/G8-1)=TRUE, "", G7/G8-1)</f>
+        <v>0.26946721311475419</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" ref="Q7:R7" si="28">IF(ISERROR(H7/H8-1)=TRUE, "", H7/H8-1)</f>
-        <v>0.32499999999999996</v>
+        <f t="shared" ref="Q7:R7" si="37">IF(ISERROR(H7/H8-1)=TRUE, "", H7/H8-1)</f>
+        <v>0.24528301886792447</v>
       </c>
       <c r="R7" s="4">
+        <f t="shared" si="37"/>
+        <v>0.71666666666666656</v>
+      </c>
+      <c r="S7" s="5">
+        <f>H7/F7</f>
+        <v>2.2095748242383664E-2</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="25"/>
+        <v>43858</v>
+      </c>
+      <c r="V7" s="14">
+        <f t="shared" si="26"/>
+        <v>17704</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="27"/>
+        <v>15858</v>
+      </c>
+      <c r="X7" s="14">
         <f t="shared" si="28"/>
-        <v>0.17647058823529416</v>
-      </c>
-      <c r="S7" s="5">
-        <f t="shared" ref="S7:S12" si="29">H7/F7</f>
-        <v>2.3477297895902548E-2</v>
-      </c>
-      <c r="U7" s="1">
-        <f t="shared" si="11"/>
-        <v>43857</v>
-      </c>
-      <c r="V7" s="14">
-        <f t="shared" si="12"/>
-        <v>15034</v>
-      </c>
-      <c r="W7" s="14">
-        <f t="shared" si="13"/>
-        <v>13679</v>
-      </c>
-      <c r="X7" s="14">
-        <f t="shared" si="14"/>
-        <v>1179</v>
+        <v>2266</v>
       </c>
       <c r="Y7" s="14">
-        <f t="shared" si="15"/>
-        <v>1771</v>
+        <f t="shared" si="29"/>
+        <v>1459</v>
       </c>
       <c r="Z7" s="14">
-        <f t="shared" si="16"/>
-        <v>515</v>
+        <f t="shared" si="30"/>
+        <v>263</v>
       </c>
       <c r="AA7" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>26</v>
       </c>
       <c r="AB7" s="14">
-        <f t="shared" si="18"/>
-        <v>9</v>
+        <f t="shared" si="32"/>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="C8" s="3">
-        <v>32799</v>
+        <v>47833</v>
       </c>
       <c r="D8" s="3">
-        <v>30453</v>
+        <v>44132</v>
       </c>
       <c r="E8" s="3">
-        <v>5794</v>
+        <v>6973</v>
       </c>
       <c r="F8" s="3">
-        <v>2744</v>
+        <v>4515</v>
       </c>
       <c r="G8" s="3">
-        <v>461</v>
+        <v>976</v>
       </c>
       <c r="H8" s="3">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="I8" s="3">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="K8" s="1">
         <f>B8</f>
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="L8" s="4">
-        <f>IF(ISERROR(C8/C9-1)=TRUE, "", C8/C9-1)</f>
-        <v>0.39981221458751226</v>
+        <f t="shared" si="13"/>
+        <v>0.45836763315954765</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" ref="M8" si="30">IF(ISERROR(D8/D9-1)=TRUE, "", D8/D9-1)</f>
-        <v>0.41273891259974027</v>
+        <f t="shared" ref="M8" si="38">IF(ISERROR(D8/D9-1)=TRUE, "", D8/D9-1)</f>
+        <v>0.44918398844120455</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" ref="N8" si="31">IF(ISERROR(E8/E9-1)=TRUE, "", E8/E9-1)</f>
-        <v>1.1587183308494784</v>
+        <f t="shared" ref="N8" si="39">IF(ISERROR(E8/E9-1)=TRUE, "", E8/E9-1)</f>
+        <v>0.20348636520538488</v>
       </c>
       <c r="O8" s="4">
-        <f t="shared" ref="O8" si="32">IF(ISERROR(F8/F9-1)=TRUE, "", F8/F9-1)</f>
-        <v>0.38936708860759484</v>
+        <f t="shared" ref="O8" si="40">IF(ISERROR(F8/F9-1)=TRUE, "", F8/F9-1)</f>
+        <v>0.64540816326530615</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" ref="P8" si="33">IF(ISERROR(G8/G9-1)=TRUE, "", G8/G9-1)</f>
-        <v>0.42283950617283961</v>
+        <f t="shared" ref="P8" si="41">IF(ISERROR(G8/G9-1)=TRUE, "", G8/G9-1)</f>
+        <v>1.1171366594360088</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" ref="Q8:R8" si="34">IF(ISERROR(H8/H9-1)=TRUE, "", H8/H9-1)</f>
-        <v>0.4285714285714286</v>
+        <f t="shared" ref="Q8:R8" si="42">IF(ISERROR(H8/H9-1)=TRUE, "", H8/H9-1)</f>
+        <v>0.32499999999999996</v>
       </c>
       <c r="R8" s="4">
-        <f t="shared" si="34"/>
-        <v>4.081632653061229E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.17647058823529416</v>
       </c>
       <c r="S8" s="5">
+        <f t="shared" ref="S8:S13" si="43">H8/F8</f>
+        <v>2.3477297895902548E-2</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="25"/>
+        <v>43857</v>
+      </c>
+      <c r="V8" s="14">
+        <f t="shared" si="26"/>
+        <v>15034</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="27"/>
+        <v>13679</v>
+      </c>
+      <c r="X8" s="14">
+        <f t="shared" si="28"/>
+        <v>1179</v>
+      </c>
+      <c r="Y8" s="14">
         <f t="shared" si="29"/>
-        <v>2.9154518950437316E-2</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="11"/>
-        <v>43856</v>
-      </c>
-      <c r="V8" s="14">
-        <f t="shared" si="12"/>
-        <v>9368</v>
-      </c>
-      <c r="W8" s="14">
-        <f t="shared" si="13"/>
-        <v>8897</v>
-      </c>
-      <c r="X8" s="14">
-        <f t="shared" si="14"/>
-        <v>3110</v>
-      </c>
-      <c r="Y8" s="14">
-        <f t="shared" si="15"/>
-        <v>769</v>
+        <v>1771</v>
       </c>
       <c r="Z8" s="14">
-        <f t="shared" si="16"/>
-        <v>137</v>
+        <f t="shared" si="30"/>
+        <v>515</v>
       </c>
       <c r="AA8" s="14">
-        <f t="shared" si="17"/>
-        <v>24</v>
+        <f t="shared" si="31"/>
+        <v>26</v>
       </c>
       <c r="AB8" s="14">
-        <f t="shared" si="18"/>
-        <v>2</v>
+        <f t="shared" si="32"/>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C9" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D9" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E9" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F9" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G9" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H9" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="I9" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K9" s="1">
-        <v>43855</v>
+        <f>B9</f>
+        <v>43856</v>
       </c>
       <c r="L9" s="4">
-        <f>IF(ISERROR(C9/C10-1)=TRUE, "", C9/C10-1)</f>
-        <v>0.54181746397315256</v>
+        <f t="shared" si="13"/>
+        <v>0.39981221458751226</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" ref="M9:R14" si="35">IF(ISERROR(D9/D10-1)=TRUE, "", D9/D10-1)</f>
-        <v>0.54335218729863244</v>
+        <f t="shared" ref="M9" si="44">IF(ISERROR(D9/D10-1)=TRUE, "", D9/D10-1)</f>
+        <v>0.41273891259974027</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="35"/>
-        <v>0.36590330788804071</v>
+        <f t="shared" ref="N9" si="45">IF(ISERROR(E9/E10-1)=TRUE, "", E9/E10-1)</f>
+        <v>1.1587183308494784</v>
       </c>
       <c r="O9" s="4">
-        <f t="shared" si="35"/>
-        <v>0.53457653457653453</v>
+        <f t="shared" ref="O9" si="46">IF(ISERROR(F9/F10-1)=TRUE, "", F9/F10-1)</f>
+        <v>0.38936708860759484</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" si="35"/>
-        <v>0.36708860759493667</v>
+        <f t="shared" ref="P9" si="47">IF(ISERROR(G9/G10-1)=TRUE, "", G9/G10-1)</f>
+        <v>0.42283950617283961</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="35"/>
-        <v>0.36585365853658547</v>
+        <f t="shared" ref="Q9:R9" si="48">IF(ISERROR(H9/H10-1)=TRUE, "", H9/H10-1)</f>
+        <v>0.4285714285714286</v>
       </c>
       <c r="R9" s="4">
-        <f t="shared" si="35"/>
-        <v>0.28947368421052633</v>
+        <f t="shared" si="48"/>
+        <v>4.081632653061229E-2</v>
       </c>
       <c r="S9" s="5">
+        <f t="shared" si="43"/>
+        <v>2.9154518950437316E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="25"/>
+        <v>43856</v>
+      </c>
+      <c r="V9" s="14">
+        <f t="shared" si="26"/>
+        <v>9368</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" si="27"/>
+        <v>8897</v>
+      </c>
+      <c r="X9" s="14">
+        <f t="shared" si="28"/>
+        <v>3110</v>
+      </c>
+      <c r="Y9" s="14">
         <f t="shared" si="29"/>
-        <v>2.8354430379746835E-2</v>
-      </c>
-      <c r="U9" s="1">
-        <f t="shared" si="11"/>
-        <v>43855</v>
-      </c>
-      <c r="V9" s="14">
-        <f t="shared" si="12"/>
-        <v>8234</v>
-      </c>
-      <c r="W9" s="14">
-        <f t="shared" si="13"/>
-        <v>7589</v>
-      </c>
-      <c r="X9" s="14">
-        <f t="shared" si="14"/>
-        <v>719</v>
-      </c>
-      <c r="Y9" s="14">
-        <f t="shared" si="15"/>
-        <v>688</v>
+        <v>769</v>
       </c>
       <c r="Z9" s="14">
-        <f t="shared" si="16"/>
-        <v>87</v>
+        <f t="shared" si="30"/>
+        <v>137</v>
       </c>
       <c r="AA9" s="14">
-        <f t="shared" si="17"/>
-        <v>15</v>
+        <f t="shared" si="31"/>
+        <v>24</v>
       </c>
       <c r="AB9" s="14">
-        <f t="shared" si="18"/>
-        <v>11</v>
+        <f t="shared" si="32"/>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="C10" s="3">
-        <v>15197</v>
+        <v>23431</v>
       </c>
       <c r="D10" s="3">
-        <v>13967</v>
+        <v>21556</v>
       </c>
       <c r="E10" s="3">
-        <v>1965</v>
+        <v>2684</v>
       </c>
       <c r="F10" s="3">
-        <v>1287</v>
+        <v>1975</v>
       </c>
       <c r="G10" s="3">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="H10" s="3">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I10" s="3">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K10" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ref="L10:L14" si="36">IF(ISERROR(C10/C11-1)=TRUE, "", C10/C11-1)</f>
-        <v>0.59850636373198696</v>
+        <f t="shared" si="13"/>
+        <v>0.54181746397315256</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.65878859857482186</v>
+        <f t="shared" ref="M10:R15" si="49">IF(ISERROR(D10/D11-1)=TRUE, "", D10/D11-1)</f>
+        <v>0.54335218729863244</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.83302238805970141</v>
+        <f t="shared" si="49"/>
+        <v>0.36590330788804071</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.55060240963855422</v>
+        <f t="shared" si="49"/>
+        <v>0.53457653457653453</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.33898305084745761</v>
+        <f t="shared" si="49"/>
+        <v>0.36708860759493667</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.6399999999999999</v>
+        <f t="shared" si="49"/>
+        <v>0.36585365853658547</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="35"/>
-        <v>0.11764705882352944</v>
+        <f t="shared" si="49"/>
+        <v>0.28947368421052633</v>
       </c>
       <c r="S10" s="5">
+        <f t="shared" si="43"/>
+        <v>2.8354430379746835E-2</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="25"/>
+        <v>43855</v>
+      </c>
+      <c r="V10" s="14">
+        <f t="shared" si="26"/>
+        <v>8234</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="27"/>
+        <v>7589</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="28"/>
+        <v>719</v>
+      </c>
+      <c r="Y10" s="14">
         <f t="shared" si="29"/>
-        <v>3.1857031857031856E-2</v>
-      </c>
-      <c r="U10" s="1">
-        <f t="shared" si="11"/>
-        <v>43854</v>
-      </c>
-      <c r="V10" s="14">
-        <f t="shared" si="12"/>
-        <v>5690</v>
-      </c>
-      <c r="W10" s="14">
-        <f t="shared" si="13"/>
-        <v>5547</v>
-      </c>
-      <c r="X10" s="14">
-        <f t="shared" si="14"/>
-        <v>893</v>
-      </c>
-      <c r="Y10" s="14">
-        <f t="shared" si="15"/>
-        <v>457</v>
+        <v>688</v>
       </c>
       <c r="Z10" s="14">
-        <f t="shared" si="16"/>
-        <v>60</v>
+        <f t="shared" si="30"/>
+        <v>87</v>
       </c>
       <c r="AA10" s="14">
-        <f t="shared" si="17"/>
-        <v>16</v>
+        <f t="shared" si="31"/>
+        <v>15</v>
       </c>
       <c r="AB10" s="14">
-        <f t="shared" si="18"/>
-        <v>4</v>
+        <f t="shared" si="32"/>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="C11" s="3">
-        <v>9507</v>
+        <v>15197</v>
       </c>
       <c r="D11" s="3">
-        <v>8420</v>
+        <v>13967</v>
       </c>
       <c r="E11" s="3">
-        <v>1072</v>
+        <v>1965</v>
       </c>
       <c r="F11" s="3">
-        <v>830</v>
+        <v>1287</v>
       </c>
       <c r="G11" s="3">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="H11" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I11" s="3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K11" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="36"/>
-        <v>0.61217568255044941</v>
+        <f t="shared" ref="L11:L15" si="50">IF(ISERROR(C11/C12-1)=TRUE, "", C11/C12-1)</f>
+        <v>0.59850636373198696</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="35"/>
-        <v>0.70860389610389607</v>
+        <f t="shared" si="49"/>
+        <v>0.65878859857482186</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="35"/>
-        <v>1.727735368956743</v>
+        <f t="shared" si="49"/>
+        <v>0.83302238805970141</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="35"/>
-        <v>0.45359019264448341</v>
+        <f t="shared" si="49"/>
+        <v>0.55060240963855422</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="35"/>
-        <v>0.86315789473684212</v>
+        <f t="shared" si="49"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="35"/>
-        <v>0.47058823529411775</v>
-      </c>
-      <c r="R11" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
+        <f t="shared" si="49"/>
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="49"/>
+        <v>0.11764705882352944</v>
       </c>
       <c r="S11" s="5">
+        <f t="shared" si="43"/>
+        <v>3.1857031857031856E-2</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="25"/>
+        <v>43854</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="26"/>
+        <v>5690</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="27"/>
+        <v>5547</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="28"/>
+        <v>893</v>
+      </c>
+      <c r="Y11" s="14">
         <f t="shared" si="29"/>
-        <v>3.0120481927710843E-2</v>
-      </c>
-      <c r="U11" s="1">
-        <f t="shared" si="11"/>
-        <v>43853</v>
-      </c>
-      <c r="V11" s="14">
-        <f t="shared" si="12"/>
-        <v>3610</v>
-      </c>
-      <c r="W11" s="14">
-        <f t="shared" si="13"/>
-        <v>3492</v>
-      </c>
-      <c r="X11" s="14">
-        <f t="shared" si="14"/>
-        <v>679</v>
-      </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="15"/>
-        <v>259</v>
+        <v>457</v>
       </c>
       <c r="Z11" s="14">
-        <f t="shared" si="16"/>
-        <v>82</v>
+        <f t="shared" si="30"/>
+        <v>60</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" si="17"/>
-        <v>8</v>
+        <f t="shared" si="31"/>
+        <v>16</v>
       </c>
       <c r="AB11" s="14">
-        <f t="shared" si="18"/>
-        <v>34</v>
+        <f t="shared" si="32"/>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="C12" s="3">
-        <v>5897</v>
+        <v>9507</v>
       </c>
       <c r="D12" s="3">
-        <v>4928</v>
+        <v>8420</v>
       </c>
       <c r="E12" s="3">
-        <v>393</v>
+        <v>1072</v>
       </c>
       <c r="F12" s="3">
-        <v>571</v>
+        <v>830</v>
       </c>
       <c r="G12" s="3">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="H12" s="3">
-        <v>17</v>
-      </c>
-      <c r="I12" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="I12" s="3">
+        <v>34</v>
+      </c>
       <c r="K12" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="36"/>
-        <v>1.6841147018661813</v>
+        <f t="shared" si="50"/>
+        <v>0.61217568255044941</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="35"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="N12" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="49"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="49"/>
+        <v>1.727735368956743</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="49"/>
+        <v>0.45359019264448341</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="49"/>
+        <v>0.86315789473684212</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="49"/>
+        <v>0.47058823529411775</v>
+      </c>
+      <c r="R12" s="4" t="str">
+        <f t="shared" si="49"/>
         <v/>
       </c>
-      <c r="O12" s="4">
-        <f t="shared" si="35"/>
-        <v>0.29772727272727262</v>
-      </c>
-      <c r="P12" s="4">
-        <f t="shared" si="35"/>
-        <v>-6.8627450980392135E-2</v>
-      </c>
-      <c r="Q12" s="4">
-        <f t="shared" si="35"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="R12" s="4"/>
       <c r="S12" s="5">
+        <f t="shared" si="43"/>
+        <v>3.0120481927710843E-2</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="25"/>
+        <v>43853</v>
+      </c>
+      <c r="V12" s="14">
+        <f t="shared" si="26"/>
+        <v>3610</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" si="27"/>
+        <v>3492</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" si="28"/>
+        <v>679</v>
+      </c>
+      <c r="Y12" s="14">
         <f t="shared" si="29"/>
-        <v>2.9772329246935202E-2</v>
-      </c>
-      <c r="U12" s="1">
-        <f t="shared" si="11"/>
-        <v>43852</v>
-      </c>
-      <c r="V12" s="14">
-        <f t="shared" si="12"/>
-        <v>3700</v>
-      </c>
-      <c r="W12" s="14">
-        <f t="shared" si="13"/>
-        <v>3534</v>
-      </c>
-      <c r="X12" s="14">
-        <f t="shared" si="14"/>
-        <v>393</v>
-      </c>
-      <c r="Y12" s="14">
-        <f t="shared" si="15"/>
-        <v>131</v>
+        <v>259</v>
       </c>
       <c r="Z12" s="14">
-        <f t="shared" si="16"/>
-        <v>-7</v>
+        <f t="shared" si="30"/>
+        <v>82</v>
       </c>
       <c r="AA12" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="AB12" s="14">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="C13" s="3">
-        <v>2197</v>
+        <v>5897</v>
       </c>
       <c r="D13" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>4928</v>
+      </c>
+      <c r="E13" s="3">
+        <v>393</v>
+      </c>
       <c r="F13" s="3">
-        <v>440</v>
+        <v>571</v>
       </c>
       <c r="G13" s="3">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H13" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I13" s="3"/>
       <c r="K13" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="36"/>
-        <v>0.26336975273145491</v>
+        <f t="shared" si="50"/>
+        <v>1.6841147018661813</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="35"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="N13" s="4">
-        <f t="shared" si="35"/>
-        <v>-1</v>
+        <f t="shared" si="49"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="N13" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
       </c>
       <c r="O13" s="4">
-        <f t="shared" si="35"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="P13" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
-      <c r="Q13" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
+        <f t="shared" si="49"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="49"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="49"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="R13" s="4"/>
+      <c r="S13" s="5">
+        <f t="shared" si="43"/>
+        <v>2.9772329246935202E-2</v>
+      </c>
       <c r="U13" s="1">
-        <f t="shared" si="11"/>
-        <v>43851</v>
-      </c>
-      <c r="V13" s="4" t="str">
-        <f t="shared" ref="V13:V14" si="37">IF(ISERROR(M13/M14-1)=TRUE, "", M13/M14-1)</f>
-        <v/>
-      </c>
-      <c r="W13" s="4" t="str">
-        <f t="shared" ref="W13:W14" si="38">IF(ISERROR(N13/N14-1)=TRUE, "", N13/N14-1)</f>
-        <v/>
-      </c>
-      <c r="X13" s="4" t="str">
-        <f t="shared" ref="X13:X14" si="39">IF(ISERROR(O13/O14-1)=TRUE, "", O13/O14-1)</f>
-        <v/>
-      </c>
-      <c r="Y13" s="4" t="str">
-        <f t="shared" ref="Y13:Y14" si="40">IF(ISERROR(P13/P14-1)=TRUE, "", P13/P14-1)</f>
-        <v/>
-      </c>
-      <c r="Z13" s="4" t="str">
-        <f t="shared" ref="Z13:Z14" si="41">IF(ISERROR(Q13/Q14-1)=TRUE, "", Q13/Q14-1)</f>
-        <v/>
-      </c>
-      <c r="AA13" s="4" t="str">
-        <f t="shared" ref="AA13:AA14" si="42">IF(ISERROR(R13/R14-1)=TRUE, "", R13/R14-1)</f>
-        <v/>
-      </c>
-      <c r="AB13" s="4"/>
+        <f t="shared" si="25"/>
+        <v>43852</v>
+      </c>
+      <c r="V13" s="14">
+        <f t="shared" si="26"/>
+        <v>3700</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="27"/>
+        <v>3534</v>
+      </c>
+      <c r="X13" s="14">
+        <f t="shared" si="28"/>
+        <v>393</v>
+      </c>
+      <c r="Y13" s="14">
+        <f t="shared" si="29"/>
+        <v>131</v>
+      </c>
+      <c r="Z13" s="14">
+        <f t="shared" si="30"/>
+        <v>-7</v>
+      </c>
+      <c r="AA13" s="14">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="AB13" s="14">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
-        <v>43850</v>
+        <v>43851</v>
       </c>
       <c r="C14" s="3">
-        <v>1739</v>
+        <v>2197</v>
       </c>
       <c r="D14" s="3">
-        <v>922</v>
-      </c>
-      <c r="E14" s="3">
-        <v>54</v>
-      </c>
+        <v>1394</v>
+      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="3">
-        <v>291</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+        <v>440</v>
+      </c>
+      <c r="G14" s="3">
+        <v>102</v>
+      </c>
+      <c r="H14" s="3">
+        <v>9</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="K14" s="1">
-        <v>43850</v>
-      </c>
-      <c r="L14" s="4" t="str">
-        <f t="shared" si="36"/>
+        <v>43851</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="50"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="49"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="49"/>
+        <v>-1</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="49"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="P14" s="4" t="str">
+        <f t="shared" si="49"/>
         <v/>
       </c>
-      <c r="M14" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
-      <c r="N14" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
-      <c r="O14" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
-      <c r="P14" s="4" t="str">
-        <f t="shared" si="35"/>
-        <v/>
-      </c>
       <c r="Q14" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="R14" s="4"/>
       <c r="U14" s="1">
-        <f t="shared" si="11"/>
-        <v>43850</v>
+        <f t="shared" si="25"/>
+        <v>43851</v>
       </c>
       <c r="V14" s="4" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="V14:V15" si="51">IF(ISERROR(M14/M15-1)=TRUE, "", M14/M15-1)</f>
         <v/>
       </c>
       <c r="W14" s="4" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="W14:W15" si="52">IF(ISERROR(N14/N15-1)=TRUE, "", N14/N15-1)</f>
         <v/>
       </c>
       <c r="X14" s="4" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="X14:X15" si="53">IF(ISERROR(O14/O15-1)=TRUE, "", O14/O15-1)</f>
         <v/>
       </c>
       <c r="Y14" s="4" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="Y14:Y15" si="54">IF(ISERROR(P14/P15-1)=TRUE, "", P14/P15-1)</f>
         <v/>
       </c>
       <c r="Z14" s="4" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="Z14:Z15" si="55">IF(ISERROR(Q14/Q15-1)=TRUE, "", Q14/Q15-1)</f>
         <v/>
       </c>
       <c r="AA14" s="4" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="AA14:AA15" si="56">IF(ISERROR(R14/R15-1)=TRUE, "", R14/R15-1)</f>
         <v/>
       </c>
       <c r="AB14" s="4"/>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="F16" s="6"/>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>43850</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1739</v>
+      </c>
+      <c r="D15" s="3">
+        <v>922</v>
+      </c>
+      <c r="E15" s="3">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3">
+        <v>291</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15" s="1">
+        <v>43850</v>
+      </c>
+      <c r="L15" s="4" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="M15" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
+      </c>
+      <c r="N15" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
+      </c>
+      <c r="O15" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
+      </c>
+      <c r="P15" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
+      </c>
+      <c r="Q15" s="4" t="str">
+        <f t="shared" si="49"/>
+        <v/>
+      </c>
+      <c r="R15" s="4"/>
+      <c r="U15" s="1">
+        <f t="shared" si="25"/>
+        <v>43850</v>
+      </c>
+      <c r="V15" s="4" t="str">
+        <f t="shared" si="51"/>
+        <v/>
+      </c>
+      <c r="W15" s="4" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="X15" s="4" t="str">
+        <f t="shared" si="53"/>
+        <v/>
+      </c>
+      <c r="Y15" s="4" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="Z15" s="4" t="str">
+        <f t="shared" si="55"/>
+        <v/>
+      </c>
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="56"/>
+        <v/>
+      </c>
+      <c r="AB15" s="4"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F17" s="6"/>
@@ -5552,6 +5703,9 @@
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F25" s="6"/>
     </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5562,7 +5716,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5591,8 +5745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673EE37A-1131-9E4A-AD70-5B0BD03BB53B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for Feb 1 data
</commit_message>
<xml_diff>
--- a/data/pandemic2020.xlsx
+++ b/data/pandemic2020.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herbyang/osmanthian/pandemic2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC33802-892C-FB41-93F3-FDB503198A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9969FF-CD8C-5E41-9AA8-655060130977}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="3120" windowWidth="27060" windowHeight="20980" activeTab="4" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
+    <workbookView xWindow="31540" yWindow="660" windowWidth="32140" windowHeight="26160" activeTab="3" xr2:uid="{68119727-28DD-F549-8437-B8BB12DD9A44}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -242,17 +242,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -421,44 +421,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -466,41 +469,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$4:$E$15</c:f>
+              <c:f>data!$E$4:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>19544</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>17988</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>15238</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>12167</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>9239</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6973</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>5794</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2684</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1965</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1072</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>393</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
@@ -541,44 +547,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -586,44 +595,47 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$4:$F$15</c:f>
+              <c:f>data!$F$4:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>14380</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>11791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>9692</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7711</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5974</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4515</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2744</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1975</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1287</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>830</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>571</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>291</c:v>
                 </c:pt>
               </c:numCache>
@@ -664,44 +676,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -709,41 +724,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$4:$G$15</c:f>
+              <c:f>data!$G$4:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>2110</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1795</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1527</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1370</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1239</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>976</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>461</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>324</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>237</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>177</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -784,44 +802,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -829,41 +850,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$4:$H$15</c:f>
+              <c:f>data!$H$4:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1248,38 +1272,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$13</c:f>
+              <c:f>data!$U$4:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1287,38 +1314,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$X$4:$X$13</c:f>
+              <c:f>data!$X$4:$X$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1556</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2750</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3071</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2928</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2266</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1179</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3110</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>719</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>893</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>679</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>393</c:v>
                 </c:pt>
               </c:numCache>
@@ -1359,38 +1389,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$13</c:f>
+              <c:f>data!$U$4:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1398,38 +1431,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$Y$4:$Y$13</c:f>
+              <c:f>data!$Y$4:$Y$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>2589</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2099</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1981</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1737</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1459</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1771</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>769</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>688</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>457</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>131</c:v>
                 </c:pt>
               </c:numCache>
@@ -1470,38 +1506,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$13</c:f>
+              <c:f>data!$U$4:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1509,38 +1548,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$Z$4:$Z$13</c:f>
+              <c:f>data!$Z$4:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>268</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>157</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>263</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>137</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>87</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>-7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1581,38 +1623,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$U$4:$U$13</c:f>
+              <c:f>data!$U$4:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
               </c:numCache>
@@ -1620,38 +1665,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$AA$4:$AA$13</c:f>
+              <c:f>data!$AA$4:$AA$14</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -2051,44 +2099,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -2096,41 +2147,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$H$4:$H$15</c:f>
+              <c:f>data!$H$4:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>259</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -2171,44 +2225,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$B$4:$B$15</c:f>
+              <c:f>data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43861</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43860</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43858</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43857</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43856</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43855</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43853</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43852</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43851</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43850</c:v>
                 </c:pt>
               </c:numCache>
@@ -2216,35 +2273,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$I$4:$I$15</c:f>
+              <c:f>data!$I$4:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>243</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>171</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>103</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
@@ -2642,7 +2702,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>259</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -6851,10 +6911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF0F35-E694-C04C-BDE8-6C99C33CAD4F}">
-  <dimension ref="B1:AB26"/>
+  <dimension ref="B1:AB27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6960,1093 +7020,1184 @@
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="C4" s="3">
-        <v>136987</v>
+        <v>163844</v>
       </c>
       <c r="D4" s="3">
-        <v>118478</v>
+        <v>137594</v>
       </c>
       <c r="E4" s="3">
-        <v>17988</v>
+        <v>19544</v>
       </c>
       <c r="F4" s="3">
-        <v>11791</v>
+        <v>14380</v>
       </c>
       <c r="G4" s="3">
-        <v>1795</v>
+        <v>2110</v>
       </c>
       <c r="H4" s="3">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="I4" s="3">
-        <v>243</v>
+        <v>328</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K9" si="0">B4</f>
-        <v>43861</v>
+        <f t="shared" ref="K4" si="0">B4</f>
+        <v>43862</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4" si="1">IF(ISERROR(C4/C5-1)=TRUE, "", C4/C5-1)</f>
-        <v>0.20609443647153092</v>
+        <v>0.19605510011898941</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4" si="2">IF(ISERROR(D4/D5-1)=TRUE, "", D4/D5-1)</f>
-        <v>0.15670672771827743</v>
+        <v>0.16134641030402275</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" ref="N4" si="3">IF(ISERROR(E4/E5-1)=TRUE, "", E4/E5-1)</f>
-        <v>0.18046987793673708</v>
+        <v>8.6502112519457386E-2</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" ref="O4" si="4">IF(ISERROR(F4/F5-1)=TRUE, "", F4/F5-1)</f>
-        <v>0.21657036731324797</v>
+        <v>0.21957425154779076</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4" si="5">IF(ISERROR(G4/G5-1)=TRUE, "", G4/G5-1)</f>
-        <v>0.17550753110674533</v>
+        <v>0.17548746518105851</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4" si="6">IF(ISERROR(H4/H5-1)=TRUE, "", H4/H5-1)</f>
-        <v>0.215962441314554</v>
+        <v>0.17374517374517384</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4" si="7">IF(ISERROR(I4/I5-1)=TRUE, "", I4/I5-1)</f>
-        <v>0.42105263157894735</v>
+        <v>0.34979423868312765</v>
       </c>
       <c r="S4" s="5">
         <f>H4/F4</f>
-        <v>2.1965906199643795E-2</v>
+        <v>2.114047287899861E-2</v>
       </c>
       <c r="U4" s="1">
         <f>K4</f>
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="V4" s="14">
         <f>C4-C5</f>
-        <v>23408</v>
+        <v>26857</v>
       </c>
       <c r="W4" s="14">
         <f t="shared" ref="W4" si="8">D4-D5</f>
-        <v>16051</v>
+        <v>19116</v>
       </c>
       <c r="X4" s="14">
         <f t="shared" ref="X4" si="9">E4-E5</f>
-        <v>2750</v>
+        <v>1556</v>
       </c>
       <c r="Y4" s="14">
         <f t="shared" ref="Y4" si="10">F4-F5</f>
-        <v>2099</v>
+        <v>2589</v>
       </c>
       <c r="Z4" s="14">
         <f t="shared" ref="Z4" si="11">G4-G5</f>
-        <v>268</v>
+        <v>315</v>
       </c>
       <c r="AA4" s="14">
         <f t="shared" ref="AA4" si="12">H4-H5</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB4" s="14">
         <f t="shared" ref="AB4" si="13">I4-I5</f>
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="C5" s="3">
-        <v>113579</v>
+        <v>136987</v>
       </c>
       <c r="D5" s="3">
-        <v>102427</v>
+        <v>118478</v>
       </c>
       <c r="E5" s="3">
-        <v>15238</v>
+        <v>17988</v>
       </c>
       <c r="F5" s="3">
-        <v>9692</v>
+        <v>11791</v>
       </c>
       <c r="G5" s="3">
-        <v>1527</v>
+        <v>1795</v>
       </c>
       <c r="H5" s="3">
-        <v>213</v>
+        <v>259</v>
       </c>
       <c r="I5" s="3">
-        <v>171</v>
+        <v>243</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="0"/>
-        <v>43860</v>
+        <f t="shared" ref="K5:K10" si="14">B5</f>
+        <v>43861</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" ref="L5:L10" si="14">IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
-        <v>0.28058584104720774</v>
+        <f t="shared" ref="L5" si="15">IF(ISERROR(C5/C6-1)=TRUE, "", C5/C6-1)</f>
+        <v>0.20609443647153092</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" ref="M5" si="15">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
-        <v>0.24991762968748099</v>
+        <f t="shared" ref="M5" si="16">IF(ISERROR(D5/D6-1)=TRUE, "", D5/D6-1)</f>
+        <v>0.15670672771827743</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" ref="N5" si="16">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
-        <v>0.25240404372482939</v>
+        <f t="shared" ref="N5" si="17">IF(ISERROR(E5/E6-1)=TRUE, "", E5/E6-1)</f>
+        <v>0.18046987793673708</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O5" si="17">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
-        <v>0.25690571910258075</v>
+        <f t="shared" ref="O5" si="18">IF(ISERROR(F5/F6-1)=TRUE, "", F5/F6-1)</f>
+        <v>0.21657036731324797</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" ref="P5" si="18">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
-        <v>0.11459854014598547</v>
+        <f t="shared" ref="P5" si="19">IF(ISERROR(G5/G6-1)=TRUE, "", G5/G6-1)</f>
+        <v>0.17550753110674533</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5:R5" si="19">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
-        <v>0.25294117647058822</v>
+        <f t="shared" ref="Q5" si="20">IF(ISERROR(H5/H6-1)=TRUE, "", H5/H6-1)</f>
+        <v>0.215962441314554</v>
       </c>
       <c r="R5" s="4">
-        <f t="shared" si="19"/>
-        <v>0.37903225806451624</v>
+        <f t="shared" ref="R5" si="21">IF(ISERROR(I5/I6-1)=TRUE, "", I5/I6-1)</f>
+        <v>0.42105263157894735</v>
       </c>
       <c r="S5" s="5">
         <f>H5/F5</f>
-        <v>2.1976888155179529E-2</v>
+        <v>2.1965906199643795E-2</v>
       </c>
       <c r="U5" s="1">
         <f>K5</f>
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="V5" s="14">
         <f>C5-C6</f>
-        <v>24886</v>
+        <v>23408</v>
       </c>
       <c r="W5" s="14">
-        <f t="shared" ref="W5:AB5" si="20">D5-D6</f>
-        <v>20480</v>
+        <f t="shared" ref="W5" si="22">D5-D6</f>
+        <v>16051</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" si="20"/>
-        <v>3071</v>
+        <f t="shared" ref="X5" si="23">E5-E6</f>
+        <v>2750</v>
       </c>
       <c r="Y5" s="14">
-        <f t="shared" si="20"/>
-        <v>1981</v>
+        <f t="shared" ref="Y5" si="24">F5-F6</f>
+        <v>2099</v>
       </c>
       <c r="Z5" s="14">
-        <f t="shared" si="20"/>
-        <v>157</v>
+        <f t="shared" ref="Z5" si="25">G5-G6</f>
+        <v>268</v>
       </c>
       <c r="AA5" s="14">
-        <f t="shared" si="20"/>
-        <v>43</v>
+        <f t="shared" ref="AA5" si="26">H5-H6</f>
+        <v>46</v>
       </c>
       <c r="AB5" s="14">
-        <f t="shared" si="20"/>
-        <v>47</v>
+        <f t="shared" ref="AB5" si="27">I5-I6</f>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>43859</v>
+        <v>43860</v>
       </c>
       <c r="C6" s="3">
-        <v>88693</v>
+        <v>113579</v>
       </c>
       <c r="D6" s="3">
-        <v>81947</v>
+        <v>102427</v>
       </c>
       <c r="E6" s="3">
-        <v>12167</v>
+        <v>15238</v>
       </c>
       <c r="F6" s="3">
-        <v>7711</v>
+        <v>9692</v>
       </c>
       <c r="G6" s="3">
-        <v>1370</v>
+        <v>1527</v>
       </c>
       <c r="H6" s="3">
-        <v>170</v>
+        <v>213</v>
       </c>
       <c r="I6" s="3">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="0"/>
-        <v>43859</v>
+        <f t="shared" si="14"/>
+        <v>43860</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="14"/>
-        <v>0.35332712818713086</v>
+        <f t="shared" ref="L6:L11" si="28">IF(ISERROR(C6/C7-1)=TRUE, "", C6/C7-1)</f>
+        <v>0.28058584104720774</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6" si="21">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
-        <v>0.36601100183363888</v>
+        <f t="shared" ref="M6" si="29">IF(ISERROR(D6/D7-1)=TRUE, "", D6/D7-1)</f>
+        <v>0.24991762968748099</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6" si="22">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
-        <v>0.31691741530468676</v>
+        <f t="shared" ref="N6" si="30">IF(ISERROR(E6/E7-1)=TRUE, "", E6/E7-1)</f>
+        <v>0.25240404372482939</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" ref="O6" si="23">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
-        <v>0.2907599598259123</v>
+        <f t="shared" ref="O6" si="31">IF(ISERROR(F6/F7-1)=TRUE, "", F6/F7-1)</f>
+        <v>0.25690571910258075</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" ref="P6" si="24">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
-        <v>0.10573042776432606</v>
+        <f t="shared" ref="P6" si="32">IF(ISERROR(G6/G7-1)=TRUE, "", G6/G7-1)</f>
+        <v>0.11459854014598547</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" ref="Q6:R6" si="25">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
-        <v>0.28787878787878785</v>
+        <f t="shared" ref="Q6:R6" si="33">IF(ISERROR(H6/H7-1)=TRUE, "", H6/H7-1)</f>
+        <v>0.25294117647058822</v>
       </c>
       <c r="R6" s="4">
-        <f t="shared" si="25"/>
-        <v>0.20388349514563098</v>
+        <f t="shared" si="33"/>
+        <v>0.37903225806451624</v>
       </c>
       <c r="S6" s="5">
         <f>H6/F6</f>
-        <v>2.2046427181947867E-2</v>
+        <v>2.1976888155179529E-2</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" ref="U6:U15" si="26">K6</f>
-        <v>43859</v>
+        <f>K6</f>
+        <v>43860</v>
       </c>
       <c r="V6" s="14">
-        <f t="shared" ref="V6:V13" si="27">C6-C7</f>
-        <v>23156</v>
+        <f>C6-C7</f>
+        <v>24886</v>
       </c>
       <c r="W6" s="14">
-        <f t="shared" ref="W6:W13" si="28">D6-D7</f>
-        <v>21957</v>
+        <f t="shared" ref="W6:AB6" si="34">D6-D7</f>
+        <v>20480</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" ref="X6:X13" si="29">E6-E7</f>
-        <v>2928</v>
+        <f t="shared" si="34"/>
+        <v>3071</v>
       </c>
       <c r="Y6" s="14">
-        <f t="shared" ref="Y6:Y13" si="30">F6-F7</f>
-        <v>1737</v>
+        <f t="shared" si="34"/>
+        <v>1981</v>
       </c>
       <c r="Z6" s="14">
-        <f t="shared" ref="Z6:Z13" si="31">G6-G7</f>
-        <v>131</v>
+        <f t="shared" si="34"/>
+        <v>157</v>
       </c>
       <c r="AA6" s="14">
-        <f t="shared" ref="AA6:AA13" si="32">H6-H7</f>
-        <v>38</v>
+        <f t="shared" si="34"/>
+        <v>43</v>
       </c>
       <c r="AB6" s="14">
-        <f t="shared" ref="AB6:AB13" si="33">I6-I7</f>
-        <v>21</v>
+        <f t="shared" si="34"/>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="C7" s="3">
-        <v>65537</v>
+        <v>88693</v>
       </c>
       <c r="D7" s="3">
-        <v>59990</v>
+        <v>81947</v>
       </c>
       <c r="E7" s="3">
-        <v>9239</v>
+        <v>12167</v>
       </c>
       <c r="F7" s="3">
-        <v>5974</v>
+        <v>7711</v>
       </c>
       <c r="G7" s="3">
-        <v>1239</v>
+        <v>1370</v>
       </c>
       <c r="H7" s="3">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="I7" s="3">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>43858</v>
+        <f t="shared" si="14"/>
+        <v>43859</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="14"/>
-        <v>0.37012104613969443</v>
+        <f t="shared" si="28"/>
+        <v>0.35332712818713086</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" ref="M7" si="34">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
-        <v>0.35933109761624227</v>
+        <f t="shared" ref="M7" si="35">IF(ISERROR(D7/D8-1)=TRUE, "", D7/D8-1)</f>
+        <v>0.36601100183363888</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" ref="N7" si="35">IF(ISERROR(E7/E8-1)=TRUE, "", E7/E8-1)</f>
-        <v>0.32496773268320656</v>
+        <f t="shared" ref="N7" si="36">IF(ISERROR(E7/E8-1)=TRUE, "", E7/E8-1)</f>
+        <v>0.31691741530468676</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" ref="O7" si="36">IF(ISERROR(F7/F8-1)=TRUE, "", F7/F8-1)</f>
-        <v>0.32314507198228126</v>
+        <f t="shared" ref="O7" si="37">IF(ISERROR(F7/F8-1)=TRUE, "", F7/F8-1)</f>
+        <v>0.2907599598259123</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" ref="P7" si="37">IF(ISERROR(G7/G8-1)=TRUE, "", G7/G8-1)</f>
-        <v>0.26946721311475419</v>
+        <f t="shared" ref="P7" si="38">IF(ISERROR(G7/G8-1)=TRUE, "", G7/G8-1)</f>
+        <v>0.10573042776432606</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" ref="Q7:R7" si="38">IF(ISERROR(H7/H8-1)=TRUE, "", H7/H8-1)</f>
-        <v>0.24528301886792447</v>
+        <f t="shared" ref="Q7:R7" si="39">IF(ISERROR(H7/H8-1)=TRUE, "", H7/H8-1)</f>
+        <v>0.28787878787878785</v>
       </c>
       <c r="R7" s="4">
-        <f t="shared" si="38"/>
-        <v>0.71666666666666656</v>
+        <f t="shared" si="39"/>
+        <v>0.20388349514563098</v>
       </c>
       <c r="S7" s="5">
         <f>H7/F7</f>
-        <v>2.2095748242383664E-2</v>
+        <v>2.2046427181947867E-2</v>
       </c>
       <c r="U7" s="1">
-        <f t="shared" si="26"/>
-        <v>43858</v>
+        <f t="shared" ref="U7:U16" si="40">K7</f>
+        <v>43859</v>
       </c>
       <c r="V7" s="14">
-        <f t="shared" si="27"/>
-        <v>17704</v>
+        <f t="shared" ref="V7:V14" si="41">C7-C8</f>
+        <v>23156</v>
       </c>
       <c r="W7" s="14">
-        <f t="shared" si="28"/>
-        <v>15858</v>
+        <f t="shared" ref="W7:W14" si="42">D7-D8</f>
+        <v>21957</v>
       </c>
       <c r="X7" s="14">
-        <f t="shared" si="29"/>
-        <v>2266</v>
+        <f t="shared" ref="X7:X14" si="43">E7-E8</f>
+        <v>2928</v>
       </c>
       <c r="Y7" s="14">
-        <f t="shared" si="30"/>
-        <v>1459</v>
+        <f t="shared" ref="Y7:Y14" si="44">F7-F8</f>
+        <v>1737</v>
       </c>
       <c r="Z7" s="14">
-        <f t="shared" si="31"/>
-        <v>263</v>
+        <f t="shared" ref="Z7:Z14" si="45">G7-G8</f>
+        <v>131</v>
       </c>
       <c r="AA7" s="14">
-        <f t="shared" si="32"/>
-        <v>26</v>
+        <f t="shared" ref="AA7:AA14" si="46">H7-H8</f>
+        <v>38</v>
       </c>
       <c r="AB7" s="14">
-        <f t="shared" si="33"/>
-        <v>43</v>
+        <f t="shared" ref="AB7:AB14" si="47">I7-I8</f>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="C8" s="3">
-        <v>47833</v>
+        <v>65537</v>
       </c>
       <c r="D8" s="3">
-        <v>44132</v>
+        <v>59990</v>
       </c>
       <c r="E8" s="3">
-        <v>6973</v>
+        <v>9239</v>
       </c>
       <c r="F8" s="3">
-        <v>4515</v>
+        <v>5974</v>
       </c>
       <c r="G8" s="3">
-        <v>976</v>
+        <v>1239</v>
       </c>
       <c r="H8" s="3">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="I8" s="3">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>43857</v>
+        <f t="shared" si="14"/>
+        <v>43858</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="14"/>
-        <v>0.45836763315954765</v>
+        <f t="shared" si="28"/>
+        <v>0.37012104613969443</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" ref="M8" si="39">IF(ISERROR(D8/D9-1)=TRUE, "", D8/D9-1)</f>
-        <v>0.44918398844120455</v>
+        <f t="shared" ref="M8" si="48">IF(ISERROR(D8/D9-1)=TRUE, "", D8/D9-1)</f>
+        <v>0.35933109761624227</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" ref="N8" si="40">IF(ISERROR(E8/E9-1)=TRUE, "", E8/E9-1)</f>
-        <v>0.20348636520538488</v>
+        <f t="shared" ref="N8" si="49">IF(ISERROR(E8/E9-1)=TRUE, "", E8/E9-1)</f>
+        <v>0.32496773268320656</v>
       </c>
       <c r="O8" s="4">
-        <f t="shared" ref="O8" si="41">IF(ISERROR(F8/F9-1)=TRUE, "", F8/F9-1)</f>
-        <v>0.64540816326530615</v>
+        <f t="shared" ref="O8" si="50">IF(ISERROR(F8/F9-1)=TRUE, "", F8/F9-1)</f>
+        <v>0.32314507198228126</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" ref="P8" si="42">IF(ISERROR(G8/G9-1)=TRUE, "", G8/G9-1)</f>
-        <v>1.1171366594360088</v>
+        <f t="shared" ref="P8" si="51">IF(ISERROR(G8/G9-1)=TRUE, "", G8/G9-1)</f>
+        <v>0.26946721311475419</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" ref="Q8:R8" si="43">IF(ISERROR(H8/H9-1)=TRUE, "", H8/H9-1)</f>
-        <v>0.32499999999999996</v>
+        <f t="shared" ref="Q8:R8" si="52">IF(ISERROR(H8/H9-1)=TRUE, "", H8/H9-1)</f>
+        <v>0.24528301886792447</v>
       </c>
       <c r="R8" s="4">
+        <f t="shared" si="52"/>
+        <v>0.71666666666666656</v>
+      </c>
+      <c r="S8" s="5">
+        <f>H8/F8</f>
+        <v>2.2095748242383664E-2</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="40"/>
+        <v>43858</v>
+      </c>
+      <c r="V8" s="14">
+        <f t="shared" si="41"/>
+        <v>17704</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="42"/>
+        <v>15858</v>
+      </c>
+      <c r="X8" s="14">
         <f t="shared" si="43"/>
-        <v>0.17647058823529416</v>
-      </c>
-      <c r="S8" s="5">
-        <f t="shared" ref="S8:S13" si="44">H8/F8</f>
-        <v>2.3477297895902548E-2</v>
-      </c>
-      <c r="U8" s="1">
-        <f t="shared" si="26"/>
-        <v>43857</v>
-      </c>
-      <c r="V8" s="14">
-        <f t="shared" si="27"/>
-        <v>15034</v>
-      </c>
-      <c r="W8" s="14">
-        <f t="shared" si="28"/>
-        <v>13679</v>
-      </c>
-      <c r="X8" s="14">
-        <f t="shared" si="29"/>
-        <v>1179</v>
+        <v>2266</v>
       </c>
       <c r="Y8" s="14">
-        <f t="shared" si="30"/>
-        <v>1771</v>
+        <f t="shared" si="44"/>
+        <v>1459</v>
       </c>
       <c r="Z8" s="14">
-        <f t="shared" si="31"/>
-        <v>515</v>
+        <f t="shared" si="45"/>
+        <v>263</v>
       </c>
       <c r="AA8" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" si="46"/>
         <v>26</v>
       </c>
       <c r="AB8" s="14">
-        <f t="shared" si="33"/>
-        <v>9</v>
+        <f t="shared" si="47"/>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="C9" s="3">
-        <v>32799</v>
+        <v>47833</v>
       </c>
       <c r="D9" s="3">
-        <v>30453</v>
+        <v>44132</v>
       </c>
       <c r="E9" s="3">
-        <v>5794</v>
+        <v>6973</v>
       </c>
       <c r="F9" s="3">
-        <v>2744</v>
+        <v>4515</v>
       </c>
       <c r="G9" s="3">
-        <v>461</v>
+        <v>976</v>
       </c>
       <c r="H9" s="3">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="I9" s="3">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="0"/>
-        <v>43856</v>
+        <f t="shared" si="14"/>
+        <v>43857</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="14"/>
-        <v>0.39981221458751226</v>
+        <f t="shared" si="28"/>
+        <v>0.45836763315954765</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" ref="M9" si="45">IF(ISERROR(D9/D10-1)=TRUE, "", D9/D10-1)</f>
-        <v>0.41273891259974027</v>
+        <f t="shared" ref="M9" si="53">IF(ISERROR(D9/D10-1)=TRUE, "", D9/D10-1)</f>
+        <v>0.44918398844120455</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" ref="N9" si="46">IF(ISERROR(E9/E10-1)=TRUE, "", E9/E10-1)</f>
-        <v>1.1587183308494784</v>
+        <f t="shared" ref="N9" si="54">IF(ISERROR(E9/E10-1)=TRUE, "", E9/E10-1)</f>
+        <v>0.20348636520538488</v>
       </c>
       <c r="O9" s="4">
-        <f t="shared" ref="O9" si="47">IF(ISERROR(F9/F10-1)=TRUE, "", F9/F10-1)</f>
-        <v>0.38936708860759484</v>
+        <f t="shared" ref="O9" si="55">IF(ISERROR(F9/F10-1)=TRUE, "", F9/F10-1)</f>
+        <v>0.64540816326530615</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" ref="P9" si="48">IF(ISERROR(G9/G10-1)=TRUE, "", G9/G10-1)</f>
-        <v>0.42283950617283961</v>
+        <f t="shared" ref="P9" si="56">IF(ISERROR(G9/G10-1)=TRUE, "", G9/G10-1)</f>
+        <v>1.1171366594360088</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" ref="Q9:R9" si="49">IF(ISERROR(H9/H10-1)=TRUE, "", H9/H10-1)</f>
-        <v>0.4285714285714286</v>
+        <f t="shared" ref="Q9:R9" si="57">IF(ISERROR(H9/H10-1)=TRUE, "", H9/H10-1)</f>
+        <v>0.32499999999999996</v>
       </c>
       <c r="R9" s="4">
-        <f t="shared" si="49"/>
-        <v>4.081632653061229E-2</v>
+        <f t="shared" si="57"/>
+        <v>0.17647058823529416</v>
       </c>
       <c r="S9" s="5">
+        <f t="shared" ref="S9:S14" si="58">H9/F9</f>
+        <v>2.3477297895902548E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="40"/>
+        <v>43857</v>
+      </c>
+      <c r="V9" s="14">
+        <f t="shared" si="41"/>
+        <v>15034</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" si="42"/>
+        <v>13679</v>
+      </c>
+      <c r="X9" s="14">
+        <f t="shared" si="43"/>
+        <v>1179</v>
+      </c>
+      <c r="Y9" s="14">
         <f t="shared" si="44"/>
-        <v>2.9154518950437316E-2</v>
-      </c>
-      <c r="U9" s="1">
-        <f t="shared" si="26"/>
-        <v>43856</v>
-      </c>
-      <c r="V9" s="14">
-        <f t="shared" si="27"/>
-        <v>9368</v>
-      </c>
-      <c r="W9" s="14">
-        <f t="shared" si="28"/>
-        <v>8897</v>
-      </c>
-      <c r="X9" s="14">
-        <f t="shared" si="29"/>
-        <v>3110</v>
-      </c>
-      <c r="Y9" s="14">
-        <f t="shared" si="30"/>
-        <v>769</v>
+        <v>1771</v>
       </c>
       <c r="Z9" s="14">
-        <f t="shared" si="31"/>
-        <v>137</v>
+        <f t="shared" si="45"/>
+        <v>515</v>
       </c>
       <c r="AA9" s="14">
-        <f t="shared" si="32"/>
-        <v>24</v>
+        <f t="shared" si="46"/>
+        <v>26</v>
       </c>
       <c r="AB9" s="14">
-        <f t="shared" si="33"/>
-        <v>2</v>
+        <f t="shared" si="47"/>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="C10" s="3">
-        <v>23431</v>
+        <v>32799</v>
       </c>
       <c r="D10" s="3">
-        <v>21556</v>
+        <v>30453</v>
       </c>
       <c r="E10" s="3">
-        <v>2684</v>
+        <v>5794</v>
       </c>
       <c r="F10" s="3">
-        <v>1975</v>
+        <v>2744</v>
       </c>
       <c r="G10" s="3">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="H10" s="3">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="I10" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K10" s="1">
-        <v>43855</v>
+        <f t="shared" si="14"/>
+        <v>43856</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="14"/>
-        <v>0.54181746397315256</v>
+        <f t="shared" si="28"/>
+        <v>0.39981221458751226</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" ref="M10:R15" si="50">IF(ISERROR(D10/D11-1)=TRUE, "", D10/D11-1)</f>
-        <v>0.54335218729863244</v>
+        <f t="shared" ref="M10" si="59">IF(ISERROR(D10/D11-1)=TRUE, "", D10/D11-1)</f>
+        <v>0.41273891259974027</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="50"/>
-        <v>0.36590330788804071</v>
+        <f t="shared" ref="N10" si="60">IF(ISERROR(E10/E11-1)=TRUE, "", E10/E11-1)</f>
+        <v>1.1587183308494784</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="50"/>
-        <v>0.53457653457653453</v>
+        <f t="shared" ref="O10" si="61">IF(ISERROR(F10/F11-1)=TRUE, "", F10/F11-1)</f>
+        <v>0.38936708860759484</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="50"/>
-        <v>0.36708860759493667</v>
+        <f t="shared" ref="P10" si="62">IF(ISERROR(G10/G11-1)=TRUE, "", G10/G11-1)</f>
+        <v>0.42283950617283961</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="50"/>
-        <v>0.36585365853658547</v>
+        <f t="shared" ref="Q10:R10" si="63">IF(ISERROR(H10/H11-1)=TRUE, "", H10/H11-1)</f>
+        <v>0.4285714285714286</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="50"/>
-        <v>0.28947368421052633</v>
+        <f t="shared" si="63"/>
+        <v>4.081632653061229E-2</v>
       </c>
       <c r="S10" s="5">
+        <f t="shared" si="58"/>
+        <v>2.9154518950437316E-2</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="40"/>
+        <v>43856</v>
+      </c>
+      <c r="V10" s="14">
+        <f t="shared" si="41"/>
+        <v>9368</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="42"/>
+        <v>8897</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="43"/>
+        <v>3110</v>
+      </c>
+      <c r="Y10" s="14">
         <f t="shared" si="44"/>
-        <v>2.8354430379746835E-2</v>
-      </c>
-      <c r="U10" s="1">
-        <f t="shared" si="26"/>
-        <v>43855</v>
-      </c>
-      <c r="V10" s="14">
-        <f t="shared" si="27"/>
-        <v>8234</v>
-      </c>
-      <c r="W10" s="14">
-        <f t="shared" si="28"/>
-        <v>7589</v>
-      </c>
-      <c r="X10" s="14">
-        <f t="shared" si="29"/>
-        <v>719</v>
-      </c>
-      <c r="Y10" s="14">
-        <f t="shared" si="30"/>
-        <v>688</v>
+        <v>769</v>
       </c>
       <c r="Z10" s="14">
-        <f t="shared" si="31"/>
-        <v>87</v>
+        <f t="shared" si="45"/>
+        <v>137</v>
       </c>
       <c r="AA10" s="14">
-        <f t="shared" si="32"/>
-        <v>15</v>
+        <f t="shared" si="46"/>
+        <v>24</v>
       </c>
       <c r="AB10" s="14">
-        <f t="shared" si="33"/>
-        <v>11</v>
+        <f t="shared" si="47"/>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="C11" s="3">
-        <v>15197</v>
+        <v>23431</v>
       </c>
       <c r="D11" s="3">
-        <v>13967</v>
+        <v>21556</v>
       </c>
       <c r="E11" s="3">
-        <v>1965</v>
+        <v>2684</v>
       </c>
       <c r="F11" s="3">
-        <v>1287</v>
+        <v>1975</v>
       </c>
       <c r="G11" s="3">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="H11" s="3">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I11" s="3">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K11" s="1">
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ref="L11:L15" si="51">IF(ISERROR(C11/C12-1)=TRUE, "", C11/C12-1)</f>
-        <v>0.59850636373198696</v>
+        <f t="shared" si="28"/>
+        <v>0.54181746397315256</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.65878859857482186</v>
+        <f t="shared" ref="M11:R16" si="64">IF(ISERROR(D11/D12-1)=TRUE, "", D11/D12-1)</f>
+        <v>0.54335218729863244</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.83302238805970141</v>
+        <f t="shared" si="64"/>
+        <v>0.36590330788804071</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.55060240963855422</v>
+        <f t="shared" si="64"/>
+        <v>0.53457653457653453</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.33898305084745761</v>
+        <f t="shared" si="64"/>
+        <v>0.36708860759493667</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.6399999999999999</v>
+        <f t="shared" si="64"/>
+        <v>0.36585365853658547</v>
       </c>
       <c r="R11" s="4">
-        <f t="shared" si="50"/>
-        <v>0.11764705882352944</v>
+        <f t="shared" si="64"/>
+        <v>0.28947368421052633</v>
       </c>
       <c r="S11" s="5">
+        <f t="shared" si="58"/>
+        <v>2.8354430379746835E-2</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="40"/>
+        <v>43855</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="41"/>
+        <v>8234</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="42"/>
+        <v>7589</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="43"/>
+        <v>719</v>
+      </c>
+      <c r="Y11" s="14">
         <f t="shared" si="44"/>
-        <v>3.1857031857031856E-2</v>
-      </c>
-      <c r="U11" s="1">
-        <f t="shared" si="26"/>
-        <v>43854</v>
-      </c>
-      <c r="V11" s="14">
-        <f t="shared" si="27"/>
-        <v>5690</v>
-      </c>
-      <c r="W11" s="14">
-        <f t="shared" si="28"/>
-        <v>5547</v>
-      </c>
-      <c r="X11" s="14">
-        <f t="shared" si="29"/>
-        <v>893</v>
-      </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="30"/>
-        <v>457</v>
+        <v>688</v>
       </c>
       <c r="Z11" s="14">
-        <f t="shared" si="31"/>
-        <v>60</v>
+        <f t="shared" si="45"/>
+        <v>87</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" si="32"/>
-        <v>16</v>
+        <f t="shared" si="46"/>
+        <v>15</v>
       </c>
       <c r="AB11" s="14">
-        <f t="shared" si="33"/>
-        <v>4</v>
+        <f t="shared" si="47"/>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="C12" s="3">
-        <v>9507</v>
+        <v>15197</v>
       </c>
       <c r="D12" s="3">
-        <v>8420</v>
+        <v>13967</v>
       </c>
       <c r="E12" s="3">
-        <v>1072</v>
+        <v>1965</v>
       </c>
       <c r="F12" s="3">
-        <v>830</v>
+        <v>1287</v>
       </c>
       <c r="G12" s="3">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="H12" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I12" s="3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="51"/>
-        <v>0.61217568255044941</v>
+        <f t="shared" ref="L12:L16" si="65">IF(ISERROR(C12/C13-1)=TRUE, "", C12/C13-1)</f>
+        <v>0.59850636373198696</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="50"/>
-        <v>0.70860389610389607</v>
+        <f t="shared" si="64"/>
+        <v>0.65878859857482186</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="50"/>
-        <v>1.727735368956743</v>
+        <f t="shared" si="64"/>
+        <v>0.83302238805970141</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="50"/>
-        <v>0.45359019264448341</v>
+        <f t="shared" si="64"/>
+        <v>0.55060240963855422</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="50"/>
-        <v>0.86315789473684212</v>
+        <f t="shared" si="64"/>
+        <v>0.33898305084745761</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="50"/>
-        <v>0.47058823529411775</v>
-      </c>
-      <c r="R12" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" si="64"/>
+        <v>0.11764705882352944</v>
       </c>
       <c r="S12" s="5">
+        <f t="shared" si="58"/>
+        <v>3.1857031857031856E-2</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="40"/>
+        <v>43854</v>
+      </c>
+      <c r="V12" s="14">
+        <f t="shared" si="41"/>
+        <v>5690</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" si="42"/>
+        <v>5547</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" si="43"/>
+        <v>893</v>
+      </c>
+      <c r="Y12" s="14">
         <f t="shared" si="44"/>
-        <v>3.0120481927710843E-2</v>
-      </c>
-      <c r="U12" s="1">
-        <f t="shared" si="26"/>
-        <v>43853</v>
-      </c>
-      <c r="V12" s="14">
-        <f t="shared" si="27"/>
-        <v>3610</v>
-      </c>
-      <c r="W12" s="14">
-        <f t="shared" si="28"/>
-        <v>3492</v>
-      </c>
-      <c r="X12" s="14">
-        <f t="shared" si="29"/>
-        <v>679</v>
-      </c>
-      <c r="Y12" s="14">
-        <f t="shared" si="30"/>
-        <v>259</v>
+        <v>457</v>
       </c>
       <c r="Z12" s="14">
-        <f t="shared" si="31"/>
-        <v>82</v>
+        <f t="shared" si="45"/>
+        <v>60</v>
       </c>
       <c r="AA12" s="14">
-        <f t="shared" si="32"/>
-        <v>8</v>
+        <f t="shared" si="46"/>
+        <v>16</v>
       </c>
       <c r="AB12" s="14">
-        <f t="shared" si="33"/>
-        <v>34</v>
+        <f t="shared" si="47"/>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="C13" s="3">
-        <v>5897</v>
+        <v>9507</v>
       </c>
       <c r="D13" s="3">
-        <v>4928</v>
+        <v>8420</v>
       </c>
       <c r="E13" s="3">
-        <v>393</v>
+        <v>1072</v>
       </c>
       <c r="F13" s="3">
-        <v>571</v>
+        <v>830</v>
       </c>
       <c r="G13" s="3">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="H13" s="3">
-        <v>17</v>
-      </c>
-      <c r="I13" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="I13" s="3">
+        <v>34</v>
+      </c>
       <c r="K13" s="1">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="51"/>
-        <v>1.6841147018661813</v>
+        <f t="shared" si="65"/>
+        <v>0.61217568255044941</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="50"/>
-        <v>2.5351506456241033</v>
-      </c>
-      <c r="N13" s="4" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="64"/>
+        <v>0.70860389610389607</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="64"/>
+        <v>1.727735368956743</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="64"/>
+        <v>0.45359019264448341</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="64"/>
+        <v>0.86315789473684212</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="64"/>
+        <v>0.47058823529411775</v>
+      </c>
+      <c r="R13" s="4" t="str">
+        <f t="shared" si="64"/>
         <v/>
       </c>
-      <c r="O13" s="4">
-        <f t="shared" si="50"/>
-        <v>0.29772727272727262</v>
-      </c>
-      <c r="P13" s="4">
-        <f t="shared" si="50"/>
-        <v>-6.8627450980392135E-2</v>
-      </c>
-      <c r="Q13" s="4">
-        <f t="shared" si="50"/>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="R13" s="4"/>
       <c r="S13" s="5">
+        <f t="shared" si="58"/>
+        <v>3.0120481927710843E-2</v>
+      </c>
+      <c r="U13" s="1">
+        <f t="shared" si="40"/>
+        <v>43853</v>
+      </c>
+      <c r="V13" s="14">
+        <f t="shared" si="41"/>
+        <v>3610</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="42"/>
+        <v>3492</v>
+      </c>
+      <c r="X13" s="14">
+        <f t="shared" si="43"/>
+        <v>679</v>
+      </c>
+      <c r="Y13" s="14">
         <f t="shared" si="44"/>
-        <v>2.9772329246935202E-2</v>
-      </c>
-      <c r="U13" s="1">
-        <f t="shared" si="26"/>
-        <v>43852</v>
-      </c>
-      <c r="V13" s="14">
-        <f t="shared" si="27"/>
-        <v>3700</v>
-      </c>
-      <c r="W13" s="14">
-        <f t="shared" si="28"/>
-        <v>3534</v>
-      </c>
-      <c r="X13" s="14">
-        <f t="shared" si="29"/>
-        <v>393</v>
-      </c>
-      <c r="Y13" s="14">
-        <f t="shared" si="30"/>
-        <v>131</v>
+        <v>259</v>
       </c>
       <c r="Z13" s="14">
-        <f t="shared" si="31"/>
-        <v>-7</v>
+        <f t="shared" si="45"/>
+        <v>82</v>
       </c>
       <c r="AA13" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" si="46"/>
         <v>8</v>
       </c>
       <c r="AB13" s="14">
-        <f t="shared" si="33"/>
-        <v>0</v>
+        <f t="shared" si="47"/>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="C14" s="3">
-        <v>2197</v>
+        <v>5897</v>
       </c>
       <c r="D14" s="3">
-        <v>1394</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>4928</v>
+      </c>
+      <c r="E14" s="3">
+        <v>393</v>
+      </c>
       <c r="F14" s="3">
-        <v>440</v>
+        <v>571</v>
       </c>
       <c r="G14" s="3">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H14" s="3">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I14" s="3"/>
       <c r="K14" s="1">
-        <v>43851</v>
+        <v>43852</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="51"/>
-        <v>0.26336975273145491</v>
+        <f t="shared" si="65"/>
+        <v>1.6841147018661813</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="50"/>
-        <v>0.51193058568329719</v>
-      </c>
-      <c r="N14" s="4">
-        <f t="shared" si="50"/>
-        <v>-1</v>
+        <f t="shared" si="64"/>
+        <v>2.5351506456241033</v>
+      </c>
+      <c r="N14" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
       </c>
       <c r="O14" s="4">
-        <f t="shared" si="50"/>
-        <v>0.51202749140893467</v>
-      </c>
-      <c r="P14" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
-      </c>
-      <c r="Q14" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
+        <f t="shared" si="64"/>
+        <v>0.29772727272727262</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="64"/>
+        <v>-6.8627450980392135E-2</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="64"/>
+        <v>0.88888888888888884</v>
       </c>
       <c r="R14" s="4"/>
+      <c r="S14" s="5">
+        <f t="shared" si="58"/>
+        <v>2.9772329246935202E-2</v>
+      </c>
       <c r="U14" s="1">
-        <f t="shared" si="26"/>
-        <v>43851</v>
-      </c>
-      <c r="V14" s="4" t="str">
-        <f t="shared" ref="V14:V15" si="52">IF(ISERROR(M14/M15-1)=TRUE, "", M14/M15-1)</f>
-        <v/>
-      </c>
-      <c r="W14" s="4" t="str">
-        <f t="shared" ref="W14:W15" si="53">IF(ISERROR(N14/N15-1)=TRUE, "", N14/N15-1)</f>
-        <v/>
-      </c>
-      <c r="X14" s="4" t="str">
-        <f t="shared" ref="X14:X15" si="54">IF(ISERROR(O14/O15-1)=TRUE, "", O14/O15-1)</f>
-        <v/>
-      </c>
-      <c r="Y14" s="4" t="str">
-        <f t="shared" ref="Y14:Y15" si="55">IF(ISERROR(P14/P15-1)=TRUE, "", P14/P15-1)</f>
-        <v/>
-      </c>
-      <c r="Z14" s="4" t="str">
-        <f t="shared" ref="Z14:Z15" si="56">IF(ISERROR(Q14/Q15-1)=TRUE, "", Q14/Q15-1)</f>
-        <v/>
-      </c>
-      <c r="AA14" s="4" t="str">
-        <f t="shared" ref="AA14:AA15" si="57">IF(ISERROR(R14/R15-1)=TRUE, "", R14/R15-1)</f>
-        <v/>
-      </c>
-      <c r="AB14" s="4"/>
+        <f t="shared" si="40"/>
+        <v>43852</v>
+      </c>
+      <c r="V14" s="14">
+        <f t="shared" si="41"/>
+        <v>3700</v>
+      </c>
+      <c r="W14" s="14">
+        <f t="shared" si="42"/>
+        <v>3534</v>
+      </c>
+      <c r="X14" s="14">
+        <f t="shared" si="43"/>
+        <v>393</v>
+      </c>
+      <c r="Y14" s="14">
+        <f t="shared" si="44"/>
+        <v>131</v>
+      </c>
+      <c r="Z14" s="14">
+        <f t="shared" si="45"/>
+        <v>-7</v>
+      </c>
+      <c r="AA14" s="14">
+        <f t="shared" si="46"/>
+        <v>8</v>
+      </c>
+      <c r="AB14" s="14">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
-        <v>43850</v>
+        <v>43851</v>
       </c>
       <c r="C15" s="3">
-        <v>1739</v>
+        <v>2197</v>
       </c>
       <c r="D15" s="3">
-        <v>922</v>
-      </c>
-      <c r="E15" s="3">
-        <v>54</v>
-      </c>
+        <v>1394</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3">
-        <v>291</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>440</v>
+      </c>
+      <c r="G15" s="3">
+        <v>102</v>
+      </c>
+      <c r="H15" s="3">
+        <v>9</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="K15" s="1">
-        <v>43850</v>
-      </c>
-      <c r="L15" s="4" t="str">
-        <f t="shared" si="51"/>
+        <v>43851</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="65"/>
+        <v>0.26336975273145491</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="64"/>
+        <v>0.51193058568329719</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="64"/>
+        <v>-1</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="64"/>
+        <v>0.51202749140893467</v>
+      </c>
+      <c r="P15" s="4" t="str">
+        <f t="shared" si="64"/>
         <v/>
       </c>
-      <c r="M15" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
-      </c>
-      <c r="N15" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
-      </c>
-      <c r="O15" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
-      </c>
-      <c r="P15" s="4" t="str">
-        <f t="shared" si="50"/>
-        <v/>
-      </c>
       <c r="Q15" s="4" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="64"/>
         <v/>
       </c>
       <c r="R15" s="4"/>
       <c r="U15" s="1">
-        <f t="shared" si="26"/>
-        <v>43850</v>
+        <f t="shared" si="40"/>
+        <v>43851</v>
       </c>
       <c r="V15" s="4" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="V15:V16" si="66">IF(ISERROR(M15/M16-1)=TRUE, "", M15/M16-1)</f>
         <v/>
       </c>
       <c r="W15" s="4" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="W15:W16" si="67">IF(ISERROR(N15/N16-1)=TRUE, "", N15/N16-1)</f>
         <v/>
       </c>
       <c r="X15" s="4" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="X15:X16" si="68">IF(ISERROR(O15/O16-1)=TRUE, "", O15/O16-1)</f>
         <v/>
       </c>
       <c r="Y15" s="4" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" ref="Y15:Y16" si="69">IF(ISERROR(P15/P16-1)=TRUE, "", P15/P16-1)</f>
         <v/>
       </c>
       <c r="Z15" s="4" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" ref="Z15:Z16" si="70">IF(ISERROR(Q15/Q16-1)=TRUE, "", Q15/Q16-1)</f>
         <v/>
       </c>
       <c r="AA15" s="4" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" ref="AA15:AA16" si="71">IF(ISERROR(R15/R16-1)=TRUE, "", R15/R16-1)</f>
         <v/>
       </c>
       <c r="AB15" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="6"/>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>43850</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1739</v>
+      </c>
+      <c r="D16" s="3">
+        <v>922</v>
+      </c>
+      <c r="E16" s="3">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3">
+        <v>291</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16" s="1">
+        <v>43850</v>
+      </c>
+      <c r="L16" s="4" t="str">
+        <f t="shared" si="65"/>
+        <v/>
+      </c>
+      <c r="M16" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
+      </c>
+      <c r="N16" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
+      </c>
+      <c r="O16" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
+      </c>
+      <c r="P16" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
+      </c>
+      <c r="Q16" s="4" t="str">
+        <f t="shared" si="64"/>
+        <v/>
+      </c>
+      <c r="R16" s="4"/>
+      <c r="U16" s="1">
+        <f t="shared" si="40"/>
+        <v>43850</v>
+      </c>
+      <c r="V16" s="4" t="str">
+        <f t="shared" si="66"/>
+        <v/>
+      </c>
+      <c r="W16" s="4" t="str">
+        <f t="shared" si="67"/>
+        <v/>
+      </c>
+      <c r="X16" s="4" t="str">
+        <f t="shared" si="68"/>
+        <v/>
+      </c>
+      <c r="Y16" s="4" t="str">
+        <f t="shared" si="69"/>
+        <v/>
+      </c>
+      <c r="Z16" s="4" t="str">
+        <f t="shared" si="70"/>
+        <v/>
+      </c>
+      <c r="AA16" s="4" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="AB16" s="4"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" s="6"/>
@@ -8074,6 +8225,9 @@
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8114,8 +8268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673EE37A-1131-9E4A-AD70-5B0BD03BB53B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8129,8 +8283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253417E2-523D-B14A-BE15-A29F328380E6}">
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8148,7 +8302,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1">
-        <f>data!B4</f>
+        <f>data!B5</f>
         <v>43861</v>
       </c>
     </row>
@@ -8167,56 +8321,56 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>data!F4</f>
-        <v>11791</v>
-      </c>
-      <c r="E6" s="19" t="s">
+        <v>14380</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E7" s="20">
+      <c r="E7" s="19">
         <v>-0.2</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="19">
         <f>-10%</f>
         <v>-0.1</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="19">
         <v>0</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="19">
         <v>0.1</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="19">
         <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <f>G8*(1+E7)</f>
-        <v>0.20379627899779762</v>
-      </c>
-      <c r="F8" s="21">
+        <v>0.18481342345696519</v>
+      </c>
+      <c r="F8" s="20">
         <f>G8*(1+F7)</f>
-        <v>0.22927081387252232</v>
-      </c>
-      <c r="G8" s="23">
+        <v>0.20791510138908584</v>
+      </c>
+      <c r="G8" s="22">
         <f>AVERAGE(data!O4:O6)</f>
-        <v>0.25474534874724702</v>
-      </c>
-      <c r="H8" s="21">
+        <v>0.23101677932120648</v>
+      </c>
+      <c r="H8" s="20">
         <f>G8*(1+H7)</f>
-        <v>0.28021988362197175</v>
-      </c>
-      <c r="I8" s="21">
+        <v>0.25411845725332716</v>
+      </c>
+      <c r="I8" s="20">
         <f>G8*(1+I7)</f>
-        <v>0.30569441849669643</v>
+        <v>0.27722013518544775</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
@@ -8235,23 +8389,23 @@
       </c>
       <c r="E10" s="3">
         <f>(1+$E$8)^D10*$D$6</f>
-        <v>43193.820116310868</v>
+        <v>47131.216289046206</v>
       </c>
       <c r="F10" s="3">
         <f>(1+$F$8)^D10*$D$6</f>
-        <v>50013.083638360324</v>
+        <v>53952.771900244159</v>
       </c>
       <c r="G10" s="3">
         <f>(1+$G$8)^D10*$D$6</f>
-        <v>57735.08380827411</v>
+        <v>61603.685392980384</v>
       </c>
       <c r="H10" s="3">
         <f>(1+$H$8)^D10*$D$6</f>
-        <v>66457.288252990722</v>
+        <v>70166.336653941267</v>
       </c>
       <c r="I10" s="3">
         <f>(1+$I$8)^D10*$D$6</f>
-        <v>76285.407892477146</v>
+        <v>79729.525896257779</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
@@ -8263,23 +8417,23 @@
       </c>
       <c r="E11" s="3">
         <f>(1+$E$8)^D11*$D$6</f>
-        <v>158231.37106608608</v>
+        <v>154475.07294053232</v>
       </c>
       <c r="F11" s="3">
         <f>(1+$F$8)^D11*$D$6</f>
-        <v>212137.09906009882</v>
+        <v>202427.09288732795</v>
       </c>
       <c r="G11" s="3">
         <f>(1+$G$8)^D11*$D$6</f>
-        <v>282702.05261202907</v>
+        <v>263909.18317088351</v>
       </c>
       <c r="H11" s="3">
         <f>(1+$H$8)^D11*$D$6</f>
-        <v>374571.38172683399</v>
+        <v>342372.37826385419</v>
       </c>
       <c r="I11" s="3">
         <f>(1+$I$8)^D11*$D$6</f>
-        <v>493551.30670185876</v>
+        <v>442058.22667886235</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
@@ -8291,23 +8445,23 @@
       </c>
       <c r="E12" s="3">
         <f>(1+$E$8)^D12*$D$6</f>
-        <v>579646.9662103093</v>
+        <v>506300.28331199015</v>
       </c>
       <c r="F12" s="3">
         <f>(1+$F$8)^D12*$D$6</f>
-        <v>899807.52082875499</v>
+        <v>759492.54304447421</v>
       </c>
       <c r="G12" s="3">
         <f>(1+$G$8)^D12*$D$6</f>
-        <v>1384261.4451977452</v>
+        <v>1130582.6350749335</v>
       </c>
       <c r="H12" s="3">
         <f>(1+$H$8)^D12*$D$6</f>
-        <v>2111186.3528743307</v>
+        <v>1670585.2263054322</v>
       </c>
       <c r="I12" s="3">
         <f>(1+$I$8)^D12*$D$6</f>
-        <v>3193178.0805373923</v>
+        <v>2450980.030017118</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
@@ -8319,23 +8473,23 @@
       </c>
       <c r="E13" s="3">
         <f>(1+$E$8)^D13*$D$6</f>
-        <v>2123413.3482701569</v>
+        <v>1659426.1585523491</v>
       </c>
       <c r="F13" s="3">
         <f>(1+$F$8)^D13*$D$6</f>
-        <v>3816652.4296187069</v>
+        <v>2849563.8341317726</v>
       </c>
       <c r="G13" s="3">
         <f>(1+$G$8)^D13*$D$6</f>
-        <v>6778089.2673271513</v>
+        <v>4843397.5634160619</v>
       </c>
       <c r="H13" s="3">
         <f>(1+$H$8)^D13*$D$6</f>
-        <v>11899221.440823473</v>
+        <v>8151519.1514636744</v>
       </c>
       <c r="I13" s="3">
         <f>(1+$I$8)^D13*$D$6</f>
-        <v>20659222.487245545</v>
+        <v>13589393.308376944</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8345,34 +8499,34 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <f>data!H4</f>
-        <v>259</v>
-      </c>
-      <c r="E16" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>-0.2</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <f>-10%</f>
         <v>-0.1</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <v>0</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <v>0.1</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -8380,25 +8534,25 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <f>G18*(1+E17)</f>
-        <v>0.20180864151038136</v>
-      </c>
-      <c r="F18" s="21">
+        <v>0.17137301107475097</v>
+      </c>
+      <c r="F18" s="20">
         <f>G18*(1+F17)</f>
-        <v>0.22703472169917902</v>
-      </c>
-      <c r="G18" s="23">
+        <v>0.19279463745909484</v>
+      </c>
+      <c r="G18" s="22">
         <f>AVERAGE(data!Q4:Q6)</f>
-        <v>0.25226080188797667</v>
-      </c>
-      <c r="H18" s="21">
+        <v>0.2142162638434387</v>
+      </c>
+      <c r="H18" s="20">
         <f>G18*(1+H17)</f>
-        <v>0.27748688207677435</v>
-      </c>
-      <c r="I18" s="21">
+        <v>0.23563789022778259</v>
+      </c>
+      <c r="I18" s="20">
         <f>G18*(1+I17)</f>
-        <v>0.30271296226557198</v>
+        <v>0.25705951661212645</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
@@ -8416,24 +8570,24 @@
         <v>7</v>
       </c>
       <c r="E20" s="3">
-        <f>$D$16*(1+E$18)^$D20</f>
-        <v>937.87945246625623</v>
+        <f t="shared" ref="E20:I23" si="0">$D$16*(1+E$18)^$D20</f>
+        <v>919.89885432165624</v>
       </c>
       <c r="F20" s="3">
-        <f>$D$16*(1+F$18)^$D20</f>
-        <v>1084.6702527875443</v>
+        <f t="shared" si="0"/>
+        <v>1044.3193602673475</v>
       </c>
       <c r="G20" s="3">
-        <f>$D$16*(1+G$18)^$D20</f>
-        <v>1250.7291448496787</v>
+        <f t="shared" si="0"/>
+        <v>1182.8942039443111</v>
       </c>
       <c r="H20" s="3">
-        <f>$D$16*(1+H$18)^$D20</f>
-        <v>1438.1192808464573</v>
+        <f t="shared" si="0"/>
+        <v>1336.9405764656135</v>
       </c>
       <c r="I20" s="3">
-        <f>$D$16*(1+I$18)^$D20</f>
-        <v>1649.0768897081923</v>
+        <f t="shared" si="0"/>
+        <v>1507.8719599944425</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
@@ -8441,28 +8595,28 @@
         <v>18</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D23" si="0">D11</f>
+        <f t="shared" ref="D21:D23" si="1">D11</f>
         <v>14</v>
       </c>
       <c r="E21" s="3">
-        <f>$D$16*(1+E$18)^$D21</f>
-        <v>3396.2079820787835</v>
+        <f t="shared" si="0"/>
+        <v>2783.5983624417622</v>
       </c>
       <c r="F21" s="3">
-        <f>$D$16*(1+F$18)^$D21</f>
-        <v>4542.5079431745016</v>
+        <f t="shared" si="0"/>
+        <v>3587.5096257539531</v>
       </c>
       <c r="G21" s="3">
-        <f>$D$16*(1+G$18)^$D21</f>
-        <v>6039.8586632293764</v>
+        <f t="shared" si="0"/>
+        <v>4602.7588740955443</v>
       </c>
       <c r="H21" s="3">
-        <f>$D$16*(1+H$18)^$D21</f>
-        <v>7985.2782468815894</v>
+        <f t="shared" si="0"/>
+        <v>5879.6385032901553</v>
       </c>
       <c r="I21" s="3">
-        <f>$D$16*(1+I$18)^$D21</f>
-        <v>10499.824664747666</v>
+        <f t="shared" si="0"/>
+        <v>7479.2034465048728</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
@@ -8470,28 +8624,28 @@
         <v>19</v>
       </c>
       <c r="D22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="E22" s="3">
-        <f>$D$16*(1+E$18)^$D22</f>
-        <v>12298.199547079452</v>
+        <v>8423.1215279664993</v>
       </c>
       <c r="F22" s="3">
-        <f>$D$16*(1+F$18)^$D22</f>
-        <v>19023.641849469172</v>
+        <f t="shared" si="0"/>
+        <v>12324.032096448418</v>
       </c>
       <c r="G22" s="3">
-        <f>$D$16*(1+G$18)^$D22</f>
-        <v>29166.900621134369</v>
+        <f t="shared" si="0"/>
+        <v>17909.792086581783</v>
       </c>
       <c r="H22" s="3">
-        <f>$D$16*(1+H$18)^$D22</f>
-        <v>44338.928995228613</v>
+        <f t="shared" si="0"/>
+        <v>25857.655559204464</v>
       </c>
       <c r="I22" s="3">
-        <f>$D$16*(1+I$18)^$D22</f>
-        <v>66853.352125959238</v>
+        <f t="shared" si="0"/>
+        <v>37097.635394995035</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
@@ -8499,28 +8653,28 @@
         <v>20</v>
       </c>
       <c r="D23">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E23" s="3">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="E23" s="3">
-        <f>$D$16*(1+E$18)^$D23</f>
-        <v>44533.70138044648</v>
+        <v>25488.22316904099</v>
       </c>
       <c r="F23" s="3">
-        <f>$D$16*(1+F$18)^$D23</f>
-        <v>79669.414725109818</v>
+        <f t="shared" si="0"/>
+        <v>42336.267483148898</v>
       </c>
       <c r="G23" s="3">
-        <f>$D$16*(1+G$18)^$D23</f>
-        <v>140849.0064547759</v>
+        <f t="shared" si="0"/>
+        <v>69688.78043771474</v>
       </c>
       <c r="H23" s="3">
-        <f>$D$16*(1+H$18)^$D23</f>
-        <v>246195.63196957653</v>
+        <f t="shared" si="0"/>
+        <v>113717.59516240819</v>
       </c>
       <c r="I23" s="3">
-        <f>$D$16*(1+I$18)^$D23</f>
-        <v>425661.45942256151</v>
+        <f t="shared" si="0"/>
+        <v>184008.17169148146</v>
       </c>
     </row>
   </sheetData>
@@ -8589,7 +8743,7 @@
       </c>
       <c r="C2" s="3">
         <f>analysis!D16</f>
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="D2" s="3">
         <v>616</v>
@@ -8630,35 +8784,35 @@
         <v>#REF!</v>
       </c>
       <c r="D3" s="3">
-        <f>D2</f>
+        <f t="shared" ref="D3:K3" si="0">D2</f>
         <v>616</v>
       </c>
       <c r="E3" s="3">
-        <f>E2</f>
+        <f t="shared" si="0"/>
         <v>2494</v>
       </c>
       <c r="F3" s="3">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>284500</v>
       </c>
       <c r="G3" s="3">
-        <f>G2</f>
+        <f t="shared" si="0"/>
         <v>774</v>
       </c>
       <c r="H3" s="3">
-        <f>H2</f>
+        <f t="shared" si="0"/>
         <v>398</v>
       </c>
       <c r="I3" s="3">
-        <f>I2</f>
+        <f t="shared" si="0"/>
         <v>455</v>
       </c>
       <c r="J3" s="3">
-        <f>J2</f>
+        <f t="shared" si="0"/>
         <v>13562</v>
       </c>
       <c r="K3" s="3">
-        <f>K2</f>
+        <f t="shared" si="0"/>
         <v>373</v>
       </c>
     </row>
@@ -8667,7 +8821,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B30" si="0">B3+1</f>
+        <f t="shared" ref="B4:B30" si="1">B3+1</f>
         <v>43863</v>
       </c>
       <c r="C4" s="3" t="e">
@@ -8675,35 +8829,35 @@
         <v>#REF!</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:K30" si="1">D3</f>
+        <f t="shared" ref="D4:K30" si="2">D3</f>
         <v>616</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8712,7 +8866,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43864</v>
       </c>
       <c r="C5" s="3" t="e">
@@ -8720,35 +8874,35 @@
         <v>#REF!</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8757,7 +8911,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43865</v>
       </c>
       <c r="C6" s="3" t="e">
@@ -8765,35 +8919,35 @@
         <v>#REF!</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8802,7 +8956,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43866</v>
       </c>
       <c r="C7" s="3" t="e">
@@ -8810,35 +8964,35 @@
         <v>#REF!</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8847,7 +9001,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43867</v>
       </c>
       <c r="C8" s="3" t="e">
@@ -8855,35 +9009,35 @@
         <v>#REF!</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8892,7 +9046,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43868</v>
       </c>
       <c r="C9" s="3" t="e">
@@ -8900,35 +9054,35 @@
         <v>#REF!</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8937,7 +9091,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43869</v>
       </c>
       <c r="C10" s="3" t="e">
@@ -8945,35 +9099,35 @@
         <v>#REF!</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -8982,7 +9136,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43870</v>
       </c>
       <c r="C11" s="3" t="e">
@@ -8990,35 +9144,35 @@
         <v>#REF!</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9027,7 +9181,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43871</v>
       </c>
       <c r="C12" s="3" t="e">
@@ -9035,35 +9189,35 @@
         <v>#REF!</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9072,7 +9226,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43872</v>
       </c>
       <c r="C13" s="3" t="e">
@@ -9080,35 +9234,35 @@
         <v>#REF!</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9117,7 +9271,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43873</v>
       </c>
       <c r="C14" s="3" t="e">
@@ -9125,35 +9279,35 @@
         <v>#REF!</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9162,7 +9316,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43874</v>
       </c>
       <c r="C15" s="3" t="e">
@@ -9170,35 +9324,35 @@
         <v>#REF!</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9207,7 +9361,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43875</v>
       </c>
       <c r="C16" s="3" t="e">
@@ -9215,35 +9369,35 @@
         <v>#REF!</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9252,7 +9406,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43876</v>
       </c>
       <c r="C17" s="3" t="e">
@@ -9260,35 +9414,35 @@
         <v>#REF!</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9297,7 +9451,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43877</v>
       </c>
       <c r="C18" s="3" t="e">
@@ -9305,35 +9459,35 @@
         <v>#REF!</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9342,7 +9496,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43878</v>
       </c>
       <c r="C19" s="3" t="e">
@@ -9350,35 +9504,35 @@
         <v>#REF!</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9387,7 +9541,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43879</v>
       </c>
       <c r="C20" s="3" t="e">
@@ -9395,35 +9549,35 @@
         <v>#REF!</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9432,7 +9586,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43880</v>
       </c>
       <c r="C21" s="3" t="e">
@@ -9440,35 +9594,35 @@
         <v>#REF!</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9477,7 +9631,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43881</v>
       </c>
       <c r="C22" s="3" t="e">
@@ -9485,35 +9639,35 @@
         <v>#REF!</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9522,7 +9676,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43882</v>
       </c>
       <c r="C23" s="3" t="e">
@@ -9530,35 +9684,35 @@
         <v>#REF!</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9567,7 +9721,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43883</v>
       </c>
       <c r="C24" s="3" t="e">
@@ -9575,35 +9729,35 @@
         <v>#REF!</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9612,7 +9766,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43884</v>
       </c>
       <c r="C25" s="3" t="e">
@@ -9620,35 +9774,35 @@
         <v>#REF!</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9657,7 +9811,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43885</v>
       </c>
       <c r="C26" s="3" t="e">
@@ -9665,35 +9819,35 @@
         <v>#REF!</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9702,7 +9856,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43886</v>
       </c>
       <c r="C27" s="3" t="e">
@@ -9710,35 +9864,35 @@
         <v>#REF!</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9747,7 +9901,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43887</v>
       </c>
       <c r="C28" s="3" t="e">
@@ -9755,35 +9909,35 @@
         <v>#REF!</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9792,7 +9946,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43888</v>
       </c>
       <c r="C29" s="3" t="e">
@@ -9800,35 +9954,35 @@
         <v>#REF!</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>
@@ -9837,7 +9991,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43889</v>
       </c>
       <c r="C30" s="3" t="e">
@@ -9845,35 +9999,35 @@
         <v>#REF!</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>616</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2494</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284500</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>774</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>455</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13562</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>373</v>
       </c>
     </row>

</xml_diff>